<commit_message>
Attaching db file and testing tables
</commit_message>
<xml_diff>
--- a/Ecommerce.xlsx
+++ b/Ecommerce.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\Proyectos_Personales\Ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E48C658-063B-42D2-8573-017383BA3E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0415AA1D-FF96-443B-9692-91451024A5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{EC1BCCFC-3DC3-41C4-92E1-54DD98A85853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{EC1BCCFC-3DC3-41C4-92E1-54DD98A85853}"/>
   </bookViews>
   <sheets>
     <sheet name="Ecommerce" sheetId="1" r:id="rId1"/>
     <sheet name="Modelacion_DB" sheetId="9" r:id="rId2"/>
-    <sheet name="register_page" sheetId="3" r:id="rId3"/>
-    <sheet name="login_page" sheetId="4" r:id="rId4"/>
-    <sheet name="main_page" sheetId="2" r:id="rId5"/>
-    <sheet name="products_page" sheetId="5" r:id="rId6"/>
-    <sheet name="individual_product_page" sheetId="6" r:id="rId7"/>
-    <sheet name="off_canvas" sheetId="7" r:id="rId8"/>
+    <sheet name="PruebaModelacionSQL" sheetId="10" r:id="rId3"/>
+    <sheet name="register_page" sheetId="3" r:id="rId4"/>
+    <sheet name="login_page" sheetId="4" r:id="rId5"/>
+    <sheet name="main_page" sheetId="2" r:id="rId6"/>
+    <sheet name="products_page" sheetId="5" r:id="rId7"/>
+    <sheet name="individual_product_page" sheetId="6" r:id="rId8"/>
+    <sheet name="off_canvas" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="285">
   <si>
     <t xml:space="preserve">Ecommerce </t>
   </si>
@@ -683,6 +684,216 @@
   </si>
   <si>
     <t>total_purchase</t>
+  </si>
+  <si>
+    <t>typeUser</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>type_name</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>autumn</t>
+  </si>
+  <si>
+    <t>sizes_value</t>
+  </si>
+  <si>
+    <t>color_name</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>dispatched</t>
+  </si>
+  <si>
+    <t>delivered</t>
+  </si>
+  <si>
+    <t>rejected</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>cristian</t>
+  </si>
+  <si>
+    <t>andres</t>
+  </si>
+  <si>
+    <t>cristian2</t>
+  </si>
+  <si>
+    <t>cristian@gmail.com</t>
+  </si>
+  <si>
+    <t>cristian2@gmail.com</t>
+  </si>
+  <si>
+    <t>alvarez2</t>
+  </si>
+  <si>
+    <t>alvarez</t>
+  </si>
+  <si>
+    <t>total_sales</t>
+  </si>
+  <si>
+    <t>total_refund</t>
+  </si>
+  <si>
+    <t>average_score</t>
+  </si>
+  <si>
+    <t>The best pants for winter</t>
+  </si>
+  <si>
+    <t>Amazing shoes for your kids</t>
+  </si>
+  <si>
+    <t>T-shirt for any person</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>quantity_articules</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>question_id</t>
+  </si>
+  <si>
+    <t>ferney</t>
+  </si>
+  <si>
+    <t>jaramillo</t>
+  </si>
+  <si>
+    <t>zapata</t>
+  </si>
+  <si>
+    <t>andres@hotmail.com</t>
+  </si>
+  <si>
+    <t>zapata@hotmail.es</t>
+  </si>
+  <si>
+    <t>¿Qué costo tiene el envio del pantalón?</t>
+  </si>
+  <si>
+    <t>¿Qué costo tiene los zapatos rojos?</t>
+  </si>
+  <si>
+    <t>Necesito comparar precios</t>
+  </si>
+  <si>
+    <t>No veo el precio en el producto</t>
+  </si>
+  <si>
+    <t>category_x_product</t>
+  </si>
+  <si>
+    <t>size_x_product</t>
+  </si>
+  <si>
+    <t>color_x_product</t>
+  </si>
+  <si>
+    <t>type_x_product_id</t>
+  </si>
+  <si>
+    <t>image_id</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/41l2imvuWJL._AC_SY395_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51Cwrg+CuVL._AC_SY395_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71FUDZ8L89L._AC_SY395_.jpg</t>
+  </si>
+  <si>
+    <t>review_id</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Your product is the best!</t>
+  </si>
+  <si>
+    <t>Terrible shop, Im not recomend this product,fuck you</t>
+  </si>
+  <si>
+    <t>answer_x_question_id</t>
+  </si>
+  <si>
+    <t>Shipping cost is free</t>
+  </si>
+  <si>
+    <t>The price is $200</t>
   </si>
 </sst>
 </file>
@@ -692,7 +903,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +958,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -769,18 +1004,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1257,11 +1492,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1304,31 +1555,22 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1336,22 +1578,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1366,38 +1608,56 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1408,46 +1668,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1455,36 +1682,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1522,9 +1719,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1902,16 +2109,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
@@ -1971,104 +2178,104 @@
     </row>
     <row r="11" spans="2:5" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="49"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="59"/>
+      <c r="C20" s="50"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="59"/>
+      <c r="C21" s="50"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="59"/>
+      <c r="C22" s="50"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="50"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="49"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -2099,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1451EF1B-7660-4F1B-AB3D-B1476CDFAB58}">
   <dimension ref="B2:K122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2115,22 +2322,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="43"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="24">
         <v>1</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C5" s="25" t="s">
@@ -2214,7 +2421,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="61" t="s">
         <v>131</v>
       </c>
       <c r="D15" s="44" t="s">
@@ -2226,516 +2433,516 @@
       <c r="F15" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="51" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="82"/>
-      <c r="D16" s="46" t="s">
+      <c r="C16" s="62"/>
+      <c r="D16" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="61"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="82"/>
-      <c r="D17" s="46" t="s">
+      <c r="C17" s="62"/>
+      <c r="D17" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="61"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="82"/>
-      <c r="D18" s="46" t="s">
+      <c r="C18" s="62"/>
+      <c r="D18" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="G18" s="61"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="82"/>
-      <c r="D19" s="46" t="s">
+      <c r="C19" s="62"/>
+      <c r="D19" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="61"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="82"/>
-      <c r="D20" s="46" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G20" s="61"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="83"/>
-      <c r="D21" s="48" t="s">
+      <c r="C21" s="63"/>
+      <c r="D21" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="62"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="53"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="63"/>
+      <c r="G22" s="54"/>
     </row>
     <row r="23" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="79"/>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="64"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="80"/>
-      <c r="D24" s="37" t="s">
+      <c r="C24" s="63"/>
+      <c r="D24" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="65"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="56"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="66" t="s">
+      <c r="G25" s="57" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="79"/>
-      <c r="D26" s="51" t="s">
+      <c r="C26" s="62"/>
+      <c r="D26" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="54"/>
-      <c r="G26" s="67"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="58"/>
     </row>
     <row r="27" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="79"/>
-      <c r="D27" s="51" t="s">
+      <c r="C27" s="62"/>
+      <c r="D27" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="54"/>
-      <c r="G27" s="67"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="58"/>
     </row>
     <row r="28" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="79"/>
-      <c r="D28" s="51" t="s">
+      <c r="C28" s="62"/>
+      <c r="D28" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="67"/>
+      <c r="G28" s="58"/>
     </row>
     <row r="29" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="79"/>
-      <c r="D29" s="51" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="51" t="s">
+      <c r="E29" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="54" t="s">
+      <c r="F29" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="67"/>
+      <c r="G29" s="58"/>
     </row>
     <row r="30" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="79"/>
-      <c r="D30" s="51" t="s">
+      <c r="C30" s="62"/>
+      <c r="D30" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="54" t="s">
+      <c r="F30" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="67"/>
+      <c r="G30" s="58"/>
     </row>
     <row r="31" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="79"/>
-      <c r="D31" s="51" t="s">
+      <c r="C31" s="62"/>
+      <c r="D31" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="54" t="s">
+      <c r="F31" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="67"/>
+      <c r="G31" s="58"/>
     </row>
     <row r="32" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="79"/>
-      <c r="D32" s="51" t="s">
+      <c r="C32" s="62"/>
+      <c r="D32" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F32" s="54" t="s">
+      <c r="F32" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="67"/>
+      <c r="G32" s="58"/>
     </row>
     <row r="33" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="79"/>
-      <c r="D33" s="51" t="s">
+      <c r="C33" s="62"/>
+      <c r="D33" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="67"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="58"/>
     </row>
     <row r="34" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="79"/>
-      <c r="D34" s="51" t="s">
+      <c r="C34" s="62"/>
+      <c r="D34" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F34" s="54" t="s">
+      <c r="F34" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="67"/>
+      <c r="G34" s="58"/>
     </row>
     <row r="35" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="79"/>
-      <c r="D35" s="51" t="s">
+      <c r="C35" s="62"/>
+      <c r="D35" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="67"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="58"/>
     </row>
     <row r="36" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="80"/>
-      <c r="D36" s="52" t="s">
+      <c r="C36" s="63"/>
+      <c r="D36" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="68"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="59"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G37" s="63"/>
+      <c r="G37" s="54"/>
     </row>
     <row r="38" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="74"/>
-      <c r="D38" s="27" t="s">
+      <c r="C38" s="68"/>
+      <c r="D38" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G38" s="64"/>
+      <c r="G38" s="55"/>
     </row>
     <row r="39" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="74"/>
-      <c r="D39" s="27" t="s">
+      <c r="C39" s="68"/>
+      <c r="D39" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="36"/>
-      <c r="G39" s="64"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="55"/>
     </row>
     <row r="40" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="75"/>
-      <c r="D40" s="37" t="s">
+      <c r="C40" s="69"/>
+      <c r="D40" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="E40" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="F40" s="38"/>
-      <c r="G40" s="65"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="56"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="78" t="s">
+      <c r="C41" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G41" s="35"/>
+      <c r="G41" s="45"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="79"/>
-      <c r="D42" s="27" t="s">
+      <c r="C42" s="62"/>
+      <c r="D42" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F42" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="36"/>
+      <c r="G42" s="46"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="79"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="62"/>
+      <c r="D43" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="27" t="s">
+      <c r="E43" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="79"/>
-      <c r="D44" s="27" t="s">
+      <c r="C44" s="62"/>
+      <c r="D44" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="27" t="s">
+      <c r="E44" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
     </row>
     <row r="45" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="80"/>
-      <c r="D45" s="37" t="s">
+      <c r="C45" s="63"/>
+      <c r="D45" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E45" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="34" t="s">
+      <c r="E46" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="35"/>
+      <c r="G46" s="45"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="79"/>
-      <c r="D47" s="27" t="s">
+      <c r="C47" s="62"/>
+      <c r="D47" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="E47" s="27" t="s">
+      <c r="E47" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F47" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G47" s="36"/>
+      <c r="G47" s="46"/>
     </row>
     <row r="48" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="80"/>
-      <c r="D48" s="37" t="s">
+      <c r="C48" s="63"/>
+      <c r="D48" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C49" s="78" t="s">
+      <c r="C49" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F49" s="35" t="s">
+      <c r="F49" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G49" s="35"/>
+      <c r="G49" s="45"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C50" s="79"/>
-      <c r="D50" s="27" t="s">
+      <c r="C50" s="62"/>
+      <c r="D50" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="27" t="s">
+      <c r="E50" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
     </row>
     <row r="51" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="80"/>
-      <c r="D51" s="37" t="s">
+      <c r="C51" s="63"/>
+      <c r="D51" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E51" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C52" s="87" t="s">
+      <c r="C52" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F52" s="53" t="s">
+      <c r="F52" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G52" s="53"/>
+      <c r="G52" s="45"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C53" s="88"/>
-      <c r="D53" s="51" t="s">
+      <c r="C53" s="62"/>
+      <c r="D53" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E53" s="51" t="s">
+      <c r="E53" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="54" t="s">
+      <c r="F53" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G53" s="54"/>
+      <c r="G53" s="46"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C54" s="88"/>
-      <c r="D54" s="51" t="s">
+      <c r="C54" s="62"/>
+      <c r="D54" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="51" t="s">
+      <c r="E54" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C55" s="88"/>
-      <c r="D55" s="51" t="s">
+      <c r="C55" s="62"/>
+      <c r="D55" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="E55" s="51" t="s">
+      <c r="E55" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F55" s="54" t="s">
+      <c r="F55" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G55" s="54"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="89"/>
-      <c r="D56" s="52" t="s">
+      <c r="C56" s="63"/>
+      <c r="D56" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="E56" s="52" t="s">
+      <c r="E56" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="23">
@@ -2766,99 +2973,99 @@
       <c r="I60" s="28"/>
     </row>
     <row r="61" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C61" s="76" t="s">
+      <c r="C61" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D61" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="E61" s="25" t="s">
+      <c r="E61" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F61" s="25" t="s">
+      <c r="F61" s="43" t="s">
         <v>97</v>
       </c>
       <c r="G61"/>
       <c r="H61" s="28"/>
     </row>
     <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C62" s="77"/>
-      <c r="D62" s="25" t="s">
+      <c r="C62" s="71"/>
+      <c r="D62" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="E62" s="25" t="s">
+      <c r="E62" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F62" s="25"/>
-      <c r="G62" s="55"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="39"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C63" s="70" t="s">
+      <c r="C63" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="E63" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F63" s="25" t="s">
+      <c r="F63" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="G63" s="56" t="s">
+      <c r="G63" s="40" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C64" s="70"/>
-      <c r="D64" s="25" t="s">
+      <c r="C64" s="64"/>
+      <c r="D64" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E64" s="25" t="s">
+      <c r="E64" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F64" s="25"/>
+      <c r="F64" s="43"/>
       <c r="H64" s="28"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C65" s="70" t="s">
+      <c r="C65" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="D65" s="25" t="s">
+      <c r="D65" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F65" s="25" t="s">
+      <c r="F65" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="G65" s="56" t="s">
+      <c r="G65" s="40" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C66" s="70"/>
-      <c r="D66" s="25" t="s">
+      <c r="C66" s="64"/>
+      <c r="D66" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E66" s="25" t="s">
+      <c r="E66" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="25"/>
+      <c r="F66" s="43"/>
       <c r="H66" s="28"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C67" s="71" t="s">
+      <c r="C67" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D67" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="E67" s="25" t="s">
+      <c r="E67" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F67" s="43" t="s">
         <v>97</v>
       </c>
       <c r="G67" s="24" t="s">
@@ -2867,50 +3074,50 @@
       <c r="I67" s="28"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C68" s="72"/>
-      <c r="D68" s="27" t="s">
+      <c r="C68" s="66"/>
+      <c r="D68" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="E68" s="25" t="s">
+      <c r="E68" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F68" s="25"/>
+      <c r="F68" s="43"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C69" s="71" t="s">
+      <c r="C69" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D69" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="E69" s="25" t="s">
+      <c r="E69" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="F69" s="43" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C70" s="72"/>
-      <c r="D70" s="27" t="s">
+      <c r="C70" s="66"/>
+      <c r="D70" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="25" t="s">
+      <c r="E70" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F70" s="25"/>
+      <c r="F70" s="43"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="71" t="s">
+      <c r="C71" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="D71" s="27" t="s">
+      <c r="D71" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="E71" s="25" t="s">
+      <c r="E71" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="F71" s="25" t="s">
+      <c r="F71" s="43" t="s">
         <v>97</v>
       </c>
       <c r="G71" s="29" t="s">
@@ -2918,14 +3125,14 @@
       </c>
     </row>
     <row r="72" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="C72" s="72"/>
-      <c r="D72" s="27" t="s">
+      <c r="C72" s="66"/>
+      <c r="D72" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="E72" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F72" s="25"/>
+      <c r="F72" s="43"/>
       <c r="G72"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
@@ -2937,697 +3144,697 @@
       </c>
     </row>
     <row r="76" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="39" t="s">
+      <c r="C76" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D76" s="39" t="s">
+      <c r="D76" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="E76" s="98" t="s">
+      <c r="E76" s="84" t="s">
         <v>177</v>
       </c>
-      <c r="F76" s="98"/>
-      <c r="G76" s="98"/>
-      <c r="H76" s="98"/>
-      <c r="I76" s="98"/>
-      <c r="J76" s="98"/>
-      <c r="K76" s="98"/>
+      <c r="F76" s="84"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="84"/>
+      <c r="I76" s="84"/>
+      <c r="J76" s="84"/>
+      <c r="K76" s="84"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C77" s="81" t="s">
+      <c r="C77" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="D77" s="44" t="s">
+      <c r="D77" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="E77" s="102"/>
-      <c r="F77" s="102"/>
-      <c r="G77" s="102"/>
-      <c r="H77" s="102"/>
-      <c r="I77" s="102"/>
-      <c r="J77" s="102"/>
-      <c r="K77" s="103"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="76"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="77"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C78" s="82"/>
-      <c r="D78" s="46" t="s">
+      <c r="C78" s="79"/>
+      <c r="D78" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="96" t="s">
+      <c r="E78" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F78" s="96"/>
-      <c r="G78" s="96"/>
-      <c r="H78" s="96"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="96"/>
-      <c r="K78" s="97"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="72"/>
+      <c r="H78" s="72"/>
+      <c r="I78" s="72"/>
+      <c r="J78" s="72"/>
+      <c r="K78" s="73"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C79" s="82"/>
-      <c r="D79" s="46" t="s">
+      <c r="C79" s="79"/>
+      <c r="D79" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="E79" s="96" t="s">
+      <c r="E79" s="72" t="s">
         <v>188</v>
       </c>
-      <c r="F79" s="96"/>
-      <c r="G79" s="96"/>
-      <c r="H79" s="96"/>
-      <c r="I79" s="96"/>
-      <c r="J79" s="96"/>
-      <c r="K79" s="97"/>
+      <c r="F79" s="72"/>
+      <c r="G79" s="72"/>
+      <c r="H79" s="72"/>
+      <c r="I79" s="72"/>
+      <c r="J79" s="72"/>
+      <c r="K79" s="73"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C80" s="82"/>
-      <c r="D80" s="46" t="s">
+      <c r="C80" s="79"/>
+      <c r="D80" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="96" t="s">
+      <c r="E80" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="F80" s="96"/>
-      <c r="G80" s="96"/>
-      <c r="H80" s="96"/>
-      <c r="I80" s="96"/>
-      <c r="J80" s="96"/>
-      <c r="K80" s="97"/>
+      <c r="F80" s="72"/>
+      <c r="G80" s="72"/>
+      <c r="H80" s="72"/>
+      <c r="I80" s="72"/>
+      <c r="J80" s="72"/>
+      <c r="K80" s="73"/>
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C81" s="86"/>
-      <c r="D81" s="46" t="s">
+      <c r="C81" s="81"/>
+      <c r="D81" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E81" s="96"/>
-      <c r="F81" s="96"/>
-      <c r="G81" s="96"/>
-      <c r="H81" s="96"/>
-      <c r="I81" s="96"/>
-      <c r="J81" s="96"/>
-      <c r="K81" s="97"/>
+      <c r="E81" s="72"/>
+      <c r="F81" s="72"/>
+      <c r="G81" s="72"/>
+      <c r="H81" s="72"/>
+      <c r="I81" s="72"/>
+      <c r="J81" s="72"/>
+      <c r="K81" s="73"/>
     </row>
     <row r="82" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="83"/>
-      <c r="D82" s="48" t="s">
+      <c r="C82" s="80"/>
+      <c r="D82" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="E82" s="104" t="s">
+      <c r="E82" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="F82" s="104"/>
-      <c r="G82" s="104"/>
-      <c r="H82" s="104"/>
-      <c r="I82" s="104"/>
-      <c r="J82" s="104"/>
-      <c r="K82" s="105"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="74"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="74"/>
+      <c r="K82" s="75"/>
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C83" s="87" t="s">
+      <c r="C83" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="D83" s="50" t="s">
+      <c r="D83" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E83" s="106" t="s">
+      <c r="E83" s="76" t="s">
         <v>209</v>
       </c>
-      <c r="F83" s="106"/>
-      <c r="G83" s="106"/>
-      <c r="H83" s="106"/>
-      <c r="I83" s="106"/>
-      <c r="J83" s="106"/>
-      <c r="K83" s="107"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
+      <c r="J83" s="76"/>
+      <c r="K83" s="77"/>
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C84" s="88"/>
-      <c r="D84" s="51" t="s">
+      <c r="C84" s="79"/>
+      <c r="D84" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="E84" s="100" t="s">
+      <c r="E84" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="F84" s="100"/>
-      <c r="G84" s="100"/>
-      <c r="H84" s="100"/>
-      <c r="I84" s="100"/>
-      <c r="J84" s="100"/>
-      <c r="K84" s="101"/>
+      <c r="F84" s="72"/>
+      <c r="G84" s="72"/>
+      <c r="H84" s="72"/>
+      <c r="I84" s="72"/>
+      <c r="J84" s="72"/>
+      <c r="K84" s="73"/>
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C85" s="88"/>
-      <c r="D85" s="51" t="s">
+      <c r="C85" s="79"/>
+      <c r="D85" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="E85" s="100" t="s">
+      <c r="E85" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="F85" s="100"/>
-      <c r="G85" s="100"/>
-      <c r="H85" s="100"/>
-      <c r="I85" s="100"/>
-      <c r="J85" s="100"/>
-      <c r="K85" s="101"/>
+      <c r="F85" s="72"/>
+      <c r="G85" s="72"/>
+      <c r="H85" s="72"/>
+      <c r="I85" s="72"/>
+      <c r="J85" s="72"/>
+      <c r="K85" s="73"/>
     </row>
     <row r="86" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="89"/>
-      <c r="D86" s="52" t="s">
+      <c r="C86" s="80"/>
+      <c r="D86" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="E86" s="108" t="s">
+      <c r="E86" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="F86" s="108"/>
-      <c r="G86" s="108"/>
-      <c r="H86" s="108"/>
-      <c r="I86" s="108"/>
-      <c r="J86" s="108"/>
-      <c r="K86" s="109"/>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="74"/>
+      <c r="I86" s="74"/>
+      <c r="J86" s="74"/>
+      <c r="K86" s="75"/>
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C87" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="D87" s="50" t="s">
+      <c r="D87" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="E87" s="106" t="s">
+      <c r="E87" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="F87" s="106"/>
-      <c r="G87" s="106"/>
-      <c r="H87" s="106"/>
-      <c r="I87" s="106"/>
-      <c r="J87" s="106"/>
-      <c r="K87" s="107"/>
+      <c r="F87" s="76"/>
+      <c r="G87" s="76"/>
+      <c r="H87" s="76"/>
+      <c r="I87" s="76"/>
+      <c r="J87" s="76"/>
+      <c r="K87" s="77"/>
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C88" s="79"/>
-      <c r="D88" s="51" t="s">
+      <c r="D88" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="E88" s="100"/>
-      <c r="F88" s="100"/>
-      <c r="G88" s="100"/>
-      <c r="H88" s="100"/>
-      <c r="I88" s="100"/>
-      <c r="J88" s="100"/>
-      <c r="K88" s="101"/>
+      <c r="E88" s="72"/>
+      <c r="F88" s="72"/>
+      <c r="G88" s="72"/>
+      <c r="H88" s="72"/>
+      <c r="I88" s="72"/>
+      <c r="J88" s="72"/>
+      <c r="K88" s="73"/>
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C89" s="79"/>
-      <c r="D89" s="51" t="s">
+      <c r="D89" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="E89" s="100"/>
-      <c r="F89" s="100"/>
-      <c r="G89" s="100"/>
-      <c r="H89" s="100"/>
-      <c r="I89" s="100"/>
-      <c r="J89" s="100"/>
-      <c r="K89" s="101"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="72"/>
+      <c r="G89" s="72"/>
+      <c r="H89" s="72"/>
+      <c r="I89" s="72"/>
+      <c r="J89" s="72"/>
+      <c r="K89" s="73"/>
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C90" s="79"/>
-      <c r="D90" s="51" t="s">
+      <c r="D90" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="E90" s="100" t="s">
+      <c r="E90" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F90" s="100"/>
-      <c r="G90" s="100"/>
-      <c r="H90" s="100"/>
-      <c r="I90" s="100"/>
-      <c r="J90" s="100"/>
-      <c r="K90" s="101"/>
+      <c r="F90" s="72"/>
+      <c r="G90" s="72"/>
+      <c r="H90" s="72"/>
+      <c r="I90" s="72"/>
+      <c r="J90" s="72"/>
+      <c r="K90" s="73"/>
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C91" s="79"/>
-      <c r="D91" s="51" t="s">
+      <c r="D91" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="100" t="s">
+      <c r="E91" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F91" s="100"/>
-      <c r="G91" s="100"/>
-      <c r="H91" s="100"/>
-      <c r="I91" s="100"/>
-      <c r="J91" s="100"/>
-      <c r="K91" s="101"/>
+      <c r="F91" s="72"/>
+      <c r="G91" s="72"/>
+      <c r="H91" s="72"/>
+      <c r="I91" s="72"/>
+      <c r="J91" s="72"/>
+      <c r="K91" s="73"/>
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C92" s="79"/>
-      <c r="D92" s="51" t="s">
+      <c r="D92" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="E92" s="100" t="s">
+      <c r="E92" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="F92" s="100"/>
-      <c r="G92" s="100"/>
-      <c r="H92" s="100"/>
-      <c r="I92" s="100"/>
-      <c r="J92" s="100"/>
-      <c r="K92" s="101"/>
+      <c r="F92" s="72"/>
+      <c r="G92" s="72"/>
+      <c r="H92" s="72"/>
+      <c r="I92" s="72"/>
+      <c r="J92" s="72"/>
+      <c r="K92" s="73"/>
     </row>
     <row r="93" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C93" s="79"/>
-      <c r="D93" s="51" t="s">
+      <c r="D93" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="E93" s="100" t="s">
+      <c r="E93" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="F93" s="100"/>
-      <c r="G93" s="100"/>
-      <c r="H93" s="100"/>
-      <c r="I93" s="100"/>
-      <c r="J93" s="100"/>
-      <c r="K93" s="101"/>
+      <c r="F93" s="72"/>
+      <c r="G93" s="72"/>
+      <c r="H93" s="72"/>
+      <c r="I93" s="72"/>
+      <c r="J93" s="72"/>
+      <c r="K93" s="73"/>
     </row>
     <row r="94" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="90"/>
+      <c r="C94" s="81"/>
       <c r="D94" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="E94" s="94" t="s">
+      <c r="E94" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="F94" s="94"/>
-      <c r="G94" s="94"/>
-      <c r="H94" s="94"/>
-      <c r="I94" s="94"/>
-      <c r="J94" s="94"/>
-      <c r="K94" s="95"/>
+      <c r="F94" s="82"/>
+      <c r="G94" s="82"/>
+      <c r="H94" s="82"/>
+      <c r="I94" s="82"/>
+      <c r="J94" s="82"/>
+      <c r="K94" s="83"/>
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C95" s="78" t="s">
         <v>201</v>
       </c>
-      <c r="D95" s="50" t="s">
+      <c r="D95" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="E95" s="106" t="s">
+      <c r="E95" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="F95" s="106"/>
-      <c r="G95" s="106"/>
-      <c r="H95" s="106"/>
-      <c r="I95" s="106"/>
-      <c r="J95" s="106"/>
-      <c r="K95" s="107"/>
+      <c r="F95" s="76"/>
+      <c r="G95" s="76"/>
+      <c r="H95" s="76"/>
+      <c r="I95" s="76"/>
+      <c r="J95" s="76"/>
+      <c r="K95" s="77"/>
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C96" s="79"/>
-      <c r="D96" s="25" t="s">
+      <c r="D96" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="E96" s="59" t="s">
+      <c r="E96" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="F96" s="59"/>
-      <c r="G96" s="59"/>
-      <c r="H96" s="59"/>
-      <c r="I96" s="59"/>
-      <c r="J96" s="59"/>
-      <c r="K96" s="91"/>
+      <c r="F96" s="72"/>
+      <c r="G96" s="72"/>
+      <c r="H96" s="72"/>
+      <c r="I96" s="72"/>
+      <c r="J96" s="72"/>
+      <c r="K96" s="73"/>
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C97" s="79"/>
-      <c r="D97" s="25" t="s">
+      <c r="D97" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="E97" s="59" t="s">
+      <c r="E97" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="F97" s="59"/>
-      <c r="G97" s="59"/>
-      <c r="H97" s="59"/>
-      <c r="I97" s="59"/>
-      <c r="J97" s="59"/>
-      <c r="K97" s="91"/>
+      <c r="F97" s="72"/>
+      <c r="G97" s="72"/>
+      <c r="H97" s="72"/>
+      <c r="I97" s="72"/>
+      <c r="J97" s="72"/>
+      <c r="K97" s="73"/>
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C98" s="79"/>
-      <c r="D98" s="25" t="s">
+      <c r="D98" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="E98" s="59" t="s">
+      <c r="E98" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="F98" s="59"/>
-      <c r="G98" s="59"/>
-      <c r="H98" s="59"/>
-      <c r="I98" s="59"/>
-      <c r="J98" s="59"/>
-      <c r="K98" s="91"/>
+      <c r="F98" s="72"/>
+      <c r="G98" s="72"/>
+      <c r="H98" s="72"/>
+      <c r="I98" s="72"/>
+      <c r="J98" s="72"/>
+      <c r="K98" s="73"/>
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C99" s="79"/>
-      <c r="D99" s="25" t="s">
+      <c r="D99" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="E99" s="59" t="s">
+      <c r="E99" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="F99" s="59"/>
-      <c r="G99" s="59"/>
-      <c r="H99" s="59"/>
-      <c r="I99" s="59"/>
-      <c r="J99" s="59"/>
-      <c r="K99" s="91"/>
+      <c r="F99" s="72"/>
+      <c r="G99" s="72"/>
+      <c r="H99" s="72"/>
+      <c r="I99" s="72"/>
+      <c r="J99" s="72"/>
+      <c r="K99" s="73"/>
     </row>
     <row r="100" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C100" s="80"/>
-      <c r="D100" s="52" t="s">
+      <c r="D100" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="E100" s="108" t="s">
+      <c r="E100" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F100" s="108"/>
-      <c r="G100" s="108"/>
-      <c r="H100" s="108"/>
-      <c r="I100" s="108"/>
-      <c r="J100" s="108"/>
-      <c r="K100" s="109"/>
+      <c r="F100" s="74"/>
+      <c r="G100" s="74"/>
+      <c r="H100" s="74"/>
+      <c r="I100" s="74"/>
+      <c r="J100" s="74"/>
+      <c r="K100" s="75"/>
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C101" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="D101" s="40" t="s">
+      <c r="D101" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="E101" s="84" t="s">
+      <c r="E101" s="76" t="s">
         <v>187</v>
       </c>
-      <c r="F101" s="84"/>
-      <c r="G101" s="84"/>
-      <c r="H101" s="84"/>
-      <c r="I101" s="84"/>
-      <c r="J101" s="84"/>
-      <c r="K101" s="85"/>
+      <c r="F101" s="76"/>
+      <c r="G101" s="76"/>
+      <c r="H101" s="76"/>
+      <c r="I101" s="76"/>
+      <c r="J101" s="76"/>
+      <c r="K101" s="77"/>
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C102" s="79"/>
-      <c r="D102" s="25" t="s">
+      <c r="D102" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="E102" s="59"/>
-      <c r="F102" s="59"/>
-      <c r="G102" s="59"/>
-      <c r="H102" s="59"/>
-      <c r="I102" s="59"/>
-      <c r="J102" s="59"/>
-      <c r="K102" s="91"/>
+      <c r="E102" s="72"/>
+      <c r="F102" s="72"/>
+      <c r="G102" s="72"/>
+      <c r="H102" s="72"/>
+      <c r="I102" s="72"/>
+      <c r="J102" s="72"/>
+      <c r="K102" s="73"/>
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C103" s="79"/>
-      <c r="D103" s="25" t="s">
+      <c r="D103" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="E103" s="59"/>
-      <c r="F103" s="59"/>
-      <c r="G103" s="59"/>
-      <c r="H103" s="59"/>
-      <c r="I103" s="59"/>
-      <c r="J103" s="59"/>
-      <c r="K103" s="91"/>
+      <c r="E103" s="72"/>
+      <c r="F103" s="72"/>
+      <c r="G103" s="72"/>
+      <c r="H103" s="72"/>
+      <c r="I103" s="72"/>
+      <c r="J103" s="72"/>
+      <c r="K103" s="73"/>
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C104" s="79"/>
-      <c r="D104" s="25" t="s">
+      <c r="D104" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="E104" s="59" t="s">
+      <c r="E104" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="F104" s="59"/>
-      <c r="G104" s="59"/>
-      <c r="H104" s="59"/>
-      <c r="I104" s="59"/>
-      <c r="J104" s="59"/>
-      <c r="K104" s="91"/>
+      <c r="F104" s="72"/>
+      <c r="G104" s="72"/>
+      <c r="H104" s="72"/>
+      <c r="I104" s="72"/>
+      <c r="J104" s="72"/>
+      <c r="K104" s="73"/>
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C105" s="79"/>
-      <c r="D105" s="25" t="s">
+      <c r="D105" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E105" s="59" t="s">
+      <c r="E105" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="F105" s="59"/>
-      <c r="G105" s="59"/>
-      <c r="H105" s="59"/>
-      <c r="I105" s="59"/>
-      <c r="J105" s="59"/>
-      <c r="K105" s="91"/>
+      <c r="F105" s="72"/>
+      <c r="G105" s="72"/>
+      <c r="H105" s="72"/>
+      <c r="I105" s="72"/>
+      <c r="J105" s="72"/>
+      <c r="K105" s="73"/>
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C106" s="79"/>
-      <c r="D106" s="25" t="s">
+      <c r="D106" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="E106" s="59"/>
-      <c r="F106" s="59"/>
-      <c r="G106" s="59"/>
-      <c r="H106" s="59"/>
-      <c r="I106" s="59"/>
-      <c r="J106" s="59"/>
-      <c r="K106" s="91"/>
+      <c r="E106" s="72"/>
+      <c r="F106" s="72"/>
+      <c r="G106" s="72"/>
+      <c r="H106" s="72"/>
+      <c r="I106" s="72"/>
+      <c r="J106" s="72"/>
+      <c r="K106" s="73"/>
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C107" s="79"/>
-      <c r="D107" s="25" t="s">
+      <c r="D107" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="E107" s="59" t="s">
+      <c r="E107" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="F107" s="59"/>
-      <c r="G107" s="59"/>
-      <c r="H107" s="59"/>
-      <c r="I107" s="59"/>
-      <c r="J107" s="59"/>
-      <c r="K107" s="91"/>
+      <c r="F107" s="72"/>
+      <c r="G107" s="72"/>
+      <c r="H107" s="72"/>
+      <c r="I107" s="72"/>
+      <c r="J107" s="72"/>
+      <c r="K107" s="73"/>
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C108" s="79"/>
-      <c r="D108" s="25" t="s">
+      <c r="D108" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="E108" s="59" t="s">
+      <c r="E108" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="59"/>
-      <c r="H108" s="59"/>
-      <c r="I108" s="59"/>
-      <c r="J108" s="59"/>
-      <c r="K108" s="91"/>
+      <c r="F108" s="72"/>
+      <c r="G108" s="72"/>
+      <c r="H108" s="72"/>
+      <c r="I108" s="72"/>
+      <c r="J108" s="72"/>
+      <c r="K108" s="73"/>
     </row>
     <row r="109" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C109" s="80"/>
-      <c r="D109" s="41" t="s">
+      <c r="D109" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E109" s="92" t="s">
+      <c r="E109" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="F109" s="92"/>
-      <c r="G109" s="92"/>
-      <c r="H109" s="92"/>
-      <c r="I109" s="92"/>
-      <c r="J109" s="92"/>
-      <c r="K109" s="93"/>
+      <c r="F109" s="74"/>
+      <c r="G109" s="74"/>
+      <c r="H109" s="74"/>
+      <c r="I109" s="74"/>
+      <c r="J109" s="74"/>
+      <c r="K109" s="75"/>
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C110" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="D110" s="40" t="s">
+      <c r="D110" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="E110" s="84" t="s">
+      <c r="E110" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="F110" s="84"/>
-      <c r="G110" s="84"/>
-      <c r="H110" s="84"/>
-      <c r="I110" s="84"/>
-      <c r="J110" s="84"/>
-      <c r="K110" s="85"/>
+      <c r="F110" s="76"/>
+      <c r="G110" s="76"/>
+      <c r="H110" s="76"/>
+      <c r="I110" s="76"/>
+      <c r="J110" s="76"/>
+      <c r="K110" s="77"/>
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C111" s="79"/>
-      <c r="D111" s="25" t="s">
+      <c r="D111" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="E111" s="59"/>
-      <c r="F111" s="59"/>
-      <c r="G111" s="59"/>
-      <c r="H111" s="59"/>
-      <c r="I111" s="59"/>
-      <c r="J111" s="59"/>
-      <c r="K111" s="91"/>
+      <c r="E111" s="72"/>
+      <c r="F111" s="72"/>
+      <c r="G111" s="72"/>
+      <c r="H111" s="72"/>
+      <c r="I111" s="72"/>
+      <c r="J111" s="72"/>
+      <c r="K111" s="73"/>
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C112" s="79"/>
-      <c r="D112" s="25" t="s">
+      <c r="D112" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="E112" s="59" t="s">
+      <c r="E112" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F112" s="59"/>
-      <c r="G112" s="59"/>
-      <c r="H112" s="59"/>
-      <c r="I112" s="59"/>
-      <c r="J112" s="59"/>
-      <c r="K112" s="91"/>
+      <c r="F112" s="72"/>
+      <c r="G112" s="72"/>
+      <c r="H112" s="72"/>
+      <c r="I112" s="72"/>
+      <c r="J112" s="72"/>
+      <c r="K112" s="73"/>
     </row>
     <row r="113" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C113" s="80"/>
-      <c r="D113" s="41" t="s">
+      <c r="D113" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E113" s="92" t="s">
+      <c r="E113" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="F113" s="92"/>
-      <c r="G113" s="92"/>
-      <c r="H113" s="92"/>
-      <c r="I113" s="92"/>
-      <c r="J113" s="92"/>
-      <c r="K113" s="93"/>
+      <c r="F113" s="74"/>
+      <c r="G113" s="74"/>
+      <c r="H113" s="74"/>
+      <c r="I113" s="74"/>
+      <c r="J113" s="74"/>
+      <c r="K113" s="75"/>
     </row>
     <row r="114" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C114" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="D114" s="40" t="s">
+      <c r="D114" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="E114" s="84" t="s">
+      <c r="E114" s="76" t="s">
         <v>185</v>
       </c>
-      <c r="F114" s="84"/>
-      <c r="G114" s="84"/>
-      <c r="H114" s="84"/>
-      <c r="I114" s="84"/>
-      <c r="J114" s="84"/>
-      <c r="K114" s="85"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
+      <c r="H114" s="76"/>
+      <c r="I114" s="76"/>
+      <c r="J114" s="76"/>
+      <c r="K114" s="77"/>
     </row>
     <row r="115" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C115" s="79"/>
-      <c r="D115" s="25" t="s">
+      <c r="D115" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="E115" s="59" t="s">
+      <c r="E115" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="F115" s="59"/>
-      <c r="G115" s="59"/>
-      <c r="H115" s="59"/>
-      <c r="I115" s="59"/>
-      <c r="J115" s="59"/>
-      <c r="K115" s="91"/>
+      <c r="F115" s="72"/>
+      <c r="G115" s="72"/>
+      <c r="H115" s="72"/>
+      <c r="I115" s="72"/>
+      <c r="J115" s="72"/>
+      <c r="K115" s="73"/>
     </row>
     <row r="116" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C116" s="79"/>
-      <c r="D116" s="25" t="s">
+      <c r="D116" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="E116" s="59" t="s">
+      <c r="E116" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="F116" s="59"/>
-      <c r="G116" s="59"/>
-      <c r="H116" s="59"/>
-      <c r="I116" s="59"/>
-      <c r="J116" s="59"/>
-      <c r="K116" s="91"/>
+      <c r="F116" s="72"/>
+      <c r="G116" s="72"/>
+      <c r="H116" s="72"/>
+      <c r="I116" s="72"/>
+      <c r="J116" s="72"/>
+      <c r="K116" s="73"/>
     </row>
     <row r="117" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C117" s="80"/>
-      <c r="D117" s="41" t="s">
+      <c r="D117" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="E117" s="92" t="s">
+      <c r="E117" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="F117" s="92"/>
-      <c r="G117" s="92"/>
-      <c r="H117" s="92"/>
-      <c r="I117" s="92"/>
-      <c r="J117" s="92"/>
-      <c r="K117" s="93"/>
+      <c r="F117" s="74"/>
+      <c r="G117" s="74"/>
+      <c r="H117" s="74"/>
+      <c r="I117" s="74"/>
+      <c r="J117" s="74"/>
+      <c r="K117" s="75"/>
     </row>
     <row r="118" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C118" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="D118" s="40" t="s">
+      <c r="D118" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E118" s="84" t="s">
+      <c r="E118" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="F118" s="84"/>
-      <c r="G118" s="84"/>
-      <c r="H118" s="84"/>
-      <c r="I118" s="84"/>
-      <c r="J118" s="84"/>
-      <c r="K118" s="85"/>
+      <c r="F118" s="76"/>
+      <c r="G118" s="76"/>
+      <c r="H118" s="76"/>
+      <c r="I118" s="76"/>
+      <c r="J118" s="76"/>
+      <c r="K118" s="77"/>
     </row>
     <row r="119" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C119" s="79"/>
-      <c r="D119" s="25" t="s">
+      <c r="D119" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="E119" s="59"/>
-      <c r="F119" s="59"/>
-      <c r="G119" s="59"/>
-      <c r="H119" s="59"/>
-      <c r="I119" s="59"/>
-      <c r="J119" s="59"/>
-      <c r="K119" s="91"/>
+      <c r="E119" s="72"/>
+      <c r="F119" s="72"/>
+      <c r="G119" s="72"/>
+      <c r="H119" s="72"/>
+      <c r="I119" s="72"/>
+      <c r="J119" s="72"/>
+      <c r="K119" s="73"/>
     </row>
     <row r="120" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C120" s="79"/>
-      <c r="D120" s="25" t="s">
+      <c r="D120" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E120" s="59" t="s">
+      <c r="E120" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="F120" s="59"/>
-      <c r="G120" s="59"/>
-      <c r="H120" s="59"/>
-      <c r="I120" s="59"/>
-      <c r="J120" s="59"/>
-      <c r="K120" s="91"/>
+      <c r="F120" s="72"/>
+      <c r="G120" s="72"/>
+      <c r="H120" s="72"/>
+      <c r="I120" s="72"/>
+      <c r="J120" s="72"/>
+      <c r="K120" s="73"/>
     </row>
     <row r="121" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C121" s="80"/>
-      <c r="D121" s="41" t="s">
+      <c r="D121" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="E121" s="92" t="s">
+      <c r="E121" s="74" t="s">
         <v>184</v>
       </c>
-      <c r="F121" s="92"/>
-      <c r="G121" s="92"/>
-      <c r="H121" s="92"/>
-      <c r="I121" s="92"/>
-      <c r="J121" s="92"/>
-      <c r="K121" s="93"/>
+      <c r="F121" s="74"/>
+      <c r="G121" s="74"/>
+      <c r="H121" s="74"/>
+      <c r="I121" s="74"/>
+      <c r="J121" s="74"/>
+      <c r="K121" s="75"/>
     </row>
     <row r="122" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C122" s="122"/>
+      <c r="C122" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="74">
@@ -3652,16 +3859,15 @@
     <mergeCell ref="E89:K89"/>
     <mergeCell ref="E90:K90"/>
     <mergeCell ref="E94:K94"/>
+    <mergeCell ref="E118:K118"/>
+    <mergeCell ref="E119:K119"/>
+    <mergeCell ref="E120:K120"/>
+    <mergeCell ref="E121:K121"/>
     <mergeCell ref="E95:K95"/>
     <mergeCell ref="E112:K112"/>
     <mergeCell ref="E113:K113"/>
     <mergeCell ref="E114:K114"/>
     <mergeCell ref="E115:K115"/>
-    <mergeCell ref="E116:K116"/>
-    <mergeCell ref="E118:K118"/>
-    <mergeCell ref="E119:K119"/>
-    <mergeCell ref="E120:K120"/>
-    <mergeCell ref="E121:K121"/>
     <mergeCell ref="E103:K103"/>
     <mergeCell ref="E104:K104"/>
     <mergeCell ref="E105:K105"/>
@@ -3669,9 +3875,6 @@
     <mergeCell ref="E107:K107"/>
     <mergeCell ref="E108:K108"/>
     <mergeCell ref="E109:K109"/>
-    <mergeCell ref="E110:K110"/>
-    <mergeCell ref="E111:K111"/>
-    <mergeCell ref="E101:K101"/>
     <mergeCell ref="C114:C117"/>
     <mergeCell ref="C118:C121"/>
     <mergeCell ref="C71:C72"/>
@@ -3681,12 +3884,16 @@
     <mergeCell ref="C87:C94"/>
     <mergeCell ref="C101:C109"/>
     <mergeCell ref="C110:C113"/>
-    <mergeCell ref="E102:K102"/>
     <mergeCell ref="E96:K96"/>
     <mergeCell ref="E97:K97"/>
     <mergeCell ref="E98:K98"/>
     <mergeCell ref="E99:K99"/>
     <mergeCell ref="E117:K117"/>
+    <mergeCell ref="E116:K116"/>
+    <mergeCell ref="E110:K110"/>
+    <mergeCell ref="E111:K111"/>
+    <mergeCell ref="E101:K101"/>
+    <mergeCell ref="E102:K102"/>
     <mergeCell ref="C63:C64"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="C67:C68"/>
@@ -3714,11 +3921,1151 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59B929-1572-41F9-B1E2-00E5AACADABB}">
+  <dimension ref="A2:N61"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="103" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="103" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="103" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="100">
+        <v>1</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="100">
+        <v>1</v>
+      </c>
+      <c r="E3" s="100" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="G3" s="101" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3" s="100">
+        <v>5555555</v>
+      </c>
+      <c r="I3" s="100">
+        <v>123456789</v>
+      </c>
+      <c r="J3" s="100">
+        <v>1</v>
+      </c>
+      <c r="K3" s="102">
+        <v>45250</v>
+      </c>
+      <c r="L3" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="100">
+        <v>2</v>
+      </c>
+      <c r="B4" s="100" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="100">
+        <v>2</v>
+      </c>
+      <c r="E4" s="100" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4" s="100" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="H4" s="100">
+        <v>2222222</v>
+      </c>
+      <c r="I4" s="100">
+        <v>123456789</v>
+      </c>
+      <c r="J4" s="100">
+        <v>2</v>
+      </c>
+      <c r="K4" s="102">
+        <v>45250</v>
+      </c>
+      <c r="L4" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="98" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="98" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="98" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" s="98" t="s">
+        <v>252</v>
+      </c>
+      <c r="L6" s="98" t="s">
+        <v>253</v>
+      </c>
+      <c r="M6" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="N6" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="100">
+        <v>1</v>
+      </c>
+      <c r="B7" s="100" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="100">
+        <v>1</v>
+      </c>
+      <c r="E7" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="100">
+        <v>100</v>
+      </c>
+      <c r="G7" s="100">
+        <v>20</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>254</v>
+      </c>
+      <c r="I7" s="100" t="s">
+        <v>257</v>
+      </c>
+      <c r="J7" s="100">
+        <v>0</v>
+      </c>
+      <c r="K7" s="100">
+        <v>0</v>
+      </c>
+      <c r="L7" s="100">
+        <v>5</v>
+      </c>
+      <c r="M7" s="102">
+        <v>45250</v>
+      </c>
+      <c r="N7" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="100">
+        <v>2</v>
+      </c>
+      <c r="B8" s="100" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="100">
+        <v>2</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="100">
+        <v>110</v>
+      </c>
+      <c r="G8" s="100">
+        <v>15</v>
+      </c>
+      <c r="H8" s="100" t="s">
+        <v>255</v>
+      </c>
+      <c r="I8" s="100" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="100">
+        <v>0</v>
+      </c>
+      <c r="K8" s="100">
+        <v>0</v>
+      </c>
+      <c r="L8" s="100">
+        <v>5</v>
+      </c>
+      <c r="M8" s="102">
+        <v>45250</v>
+      </c>
+      <c r="N8" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="100">
+        <v>3</v>
+      </c>
+      <c r="B9" s="100" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="100">
+        <v>3</v>
+      </c>
+      <c r="E9" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="100">
+        <v>80</v>
+      </c>
+      <c r="G9" s="100">
+        <v>20</v>
+      </c>
+      <c r="H9" s="100" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" s="100" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" s="100">
+        <v>0</v>
+      </c>
+      <c r="K9" s="100">
+        <v>0</v>
+      </c>
+      <c r="L9" s="100">
+        <v>5</v>
+      </c>
+      <c r="M9" s="102">
+        <v>45250</v>
+      </c>
+      <c r="N9" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="103" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="103" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" s="103" t="s">
+        <v>235</v>
+      </c>
+      <c r="H11" s="103" t="s">
+        <v>259</v>
+      </c>
+      <c r="I11" s="103" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="K11" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="100">
+        <v>1</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="100">
+        <v>1</v>
+      </c>
+      <c r="E12" s="100">
+        <v>2</v>
+      </c>
+      <c r="F12" s="100">
+        <v>200</v>
+      </c>
+      <c r="G12" s="100">
+        <v>1</v>
+      </c>
+      <c r="H12" s="100">
+        <v>1</v>
+      </c>
+      <c r="I12" s="100">
+        <v>1</v>
+      </c>
+      <c r="J12" s="102">
+        <v>45250</v>
+      </c>
+      <c r="K12" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="100">
+        <v>2</v>
+      </c>
+      <c r="B13" s="100" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="100">
+        <v>2</v>
+      </c>
+      <c r="E13" s="100">
+        <v>1</v>
+      </c>
+      <c r="F13" s="100">
+        <v>100</v>
+      </c>
+      <c r="G13" s="100">
+        <v>1</v>
+      </c>
+      <c r="H13" s="100">
+        <v>2</v>
+      </c>
+      <c r="I13" s="100">
+        <v>2</v>
+      </c>
+      <c r="J13" s="102">
+        <v>45250</v>
+      </c>
+      <c r="K13" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="100">
+        <v>3</v>
+      </c>
+      <c r="B14" s="100" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="100">
+        <v>4</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="103" t="s">
+        <v>260</v>
+      </c>
+      <c r="E15" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="103" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="103" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="103" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="L15" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D16" s="100">
+        <v>1</v>
+      </c>
+      <c r="E16" s="100" t="s">
+        <v>245</v>
+      </c>
+      <c r="F16" s="100" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="101" t="s">
+        <v>264</v>
+      </c>
+      <c r="H16" s="100">
+        <v>4444444</v>
+      </c>
+      <c r="I16" s="100" t="s">
+        <v>266</v>
+      </c>
+      <c r="J16" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="K16" s="102">
+        <v>45250</v>
+      </c>
+      <c r="L16" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="100">
+        <v>2</v>
+      </c>
+      <c r="E17" s="100" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" s="100" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" s="101" t="s">
+        <v>265</v>
+      </c>
+      <c r="H17" s="100">
+        <v>777777</v>
+      </c>
+      <c r="I17" s="100" t="s">
+        <v>267</v>
+      </c>
+      <c r="J17" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="K17" s="102">
+        <v>45250</v>
+      </c>
+      <c r="L17" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="100">
+        <v>1</v>
+      </c>
+      <c r="B18" s="100">
+        <v>35</v>
+      </c>
+      <c r="G18" s="104"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="100">
+        <v>2</v>
+      </c>
+      <c r="B19" s="100">
+        <v>36</v>
+      </c>
+      <c r="D19" s="98" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="100">
+        <v>3</v>
+      </c>
+      <c r="B20" s="100">
+        <v>37</v>
+      </c>
+      <c r="D20" s="100">
+        <v>1</v>
+      </c>
+      <c r="E20" s="100">
+        <v>1</v>
+      </c>
+      <c r="F20" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="100">
+        <v>4</v>
+      </c>
+      <c r="B21" s="100">
+        <v>38</v>
+      </c>
+      <c r="D21" s="100">
+        <v>2</v>
+      </c>
+      <c r="E21" s="100">
+        <v>2</v>
+      </c>
+      <c r="F21" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="100">
+        <v>5</v>
+      </c>
+      <c r="B22" s="100">
+        <v>39</v>
+      </c>
+      <c r="D22" s="100">
+        <v>3</v>
+      </c>
+      <c r="E22" s="100">
+        <v>3</v>
+      </c>
+      <c r="F22" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="100">
+        <v>6</v>
+      </c>
+      <c r="B23" s="100">
+        <v>40</v>
+      </c>
+      <c r="D23" s="100">
+        <v>4</v>
+      </c>
+      <c r="E23" s="100">
+        <v>4</v>
+      </c>
+      <c r="F23" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="100">
+        <v>7</v>
+      </c>
+      <c r="B24" s="100">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="100">
+        <v>8</v>
+      </c>
+      <c r="B25" s="100">
+        <v>42</v>
+      </c>
+      <c r="D25" s="98" t="s">
+        <v>271</v>
+      </c>
+      <c r="E25" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="100">
+        <v>1</v>
+      </c>
+      <c r="E26" s="100">
+        <v>1</v>
+      </c>
+      <c r="F26" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="99" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" s="100">
+        <v>2</v>
+      </c>
+      <c r="E27" s="100">
+        <v>2</v>
+      </c>
+      <c r="F27" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="100">
+        <v>1</v>
+      </c>
+      <c r="B28" s="100" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="100">
+        <v>3</v>
+      </c>
+      <c r="E28" s="100">
+        <v>3</v>
+      </c>
+      <c r="F28" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="100">
+        <v>2</v>
+      </c>
+      <c r="B29" s="100" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="100">
+        <v>4</v>
+      </c>
+      <c r="E29" s="100">
+        <v>6</v>
+      </c>
+      <c r="F29" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="100">
+        <v>3</v>
+      </c>
+      <c r="B30" s="100" t="s">
+        <v>230</v>
+      </c>
+      <c r="D30" s="100">
+        <v>5</v>
+      </c>
+      <c r="E30" s="100">
+        <v>8</v>
+      </c>
+      <c r="F30" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="100">
+        <v>4</v>
+      </c>
+      <c r="B31" s="100" t="s">
+        <v>231</v>
+      </c>
+      <c r="D31" s="100">
+        <v>6</v>
+      </c>
+      <c r="E31" s="100">
+        <v>2</v>
+      </c>
+      <c r="F31" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="100">
+        <v>5</v>
+      </c>
+      <c r="B32" s="100" t="s">
+        <v>232</v>
+      </c>
+      <c r="D32" s="100">
+        <v>7</v>
+      </c>
+      <c r="E32" s="100">
+        <v>3</v>
+      </c>
+      <c r="F32" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="100">
+        <v>6</v>
+      </c>
+      <c r="B33" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" s="100">
+        <v>8</v>
+      </c>
+      <c r="E33" s="100">
+        <v>7</v>
+      </c>
+      <c r="F33" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="100">
+        <v>7</v>
+      </c>
+      <c r="B34" s="100" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="99" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="D36" s="100">
+        <v>1</v>
+      </c>
+      <c r="E36" s="100">
+        <v>1</v>
+      </c>
+      <c r="F36" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="100">
+        <v>1</v>
+      </c>
+      <c r="B37" s="100" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" s="100">
+        <v>2</v>
+      </c>
+      <c r="E37" s="100">
+        <v>2</v>
+      </c>
+      <c r="F37" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="100">
+        <v>2</v>
+      </c>
+      <c r="B38" s="100" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" s="100">
+        <v>3</v>
+      </c>
+      <c r="E38" s="100">
+        <v>5</v>
+      </c>
+      <c r="F38" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="100">
+        <v>3</v>
+      </c>
+      <c r="B39" s="100" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="100">
+        <v>4</v>
+      </c>
+      <c r="E39" s="100">
+        <v>2</v>
+      </c>
+      <c r="F39" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="100">
+        <v>4</v>
+      </c>
+      <c r="B40" s="100" t="s">
+        <v>240</v>
+      </c>
+      <c r="D40" s="100">
+        <v>5</v>
+      </c>
+      <c r="E40" s="100">
+        <v>5</v>
+      </c>
+      <c r="F40" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="100">
+        <v>5</v>
+      </c>
+      <c r="B41" s="100" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" s="100">
+        <v>6</v>
+      </c>
+      <c r="E41" s="100">
+        <v>7</v>
+      </c>
+      <c r="F41" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="E43" s="98" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="100">
+        <v>1</v>
+      </c>
+      <c r="E44" s="100">
+        <v>1</v>
+      </c>
+      <c r="F44" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="100">
+        <v>2</v>
+      </c>
+      <c r="E45" s="100">
+        <v>2</v>
+      </c>
+      <c r="F45" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="100">
+        <v>3</v>
+      </c>
+      <c r="E46" s="100">
+        <v>3</v>
+      </c>
+      <c r="F46" s="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="100">
+        <v>4</v>
+      </c>
+      <c r="E47" s="100">
+        <v>2</v>
+      </c>
+      <c r="F47" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="100">
+        <v>5</v>
+      </c>
+      <c r="E48" s="100">
+        <v>3</v>
+      </c>
+      <c r="F48" s="100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="98" t="s">
+        <v>274</v>
+      </c>
+      <c r="E50" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="H50" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="100">
+        <v>1</v>
+      </c>
+      <c r="E51" s="100" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="100">
+        <v>1</v>
+      </c>
+      <c r="G51" s="102">
+        <v>45250</v>
+      </c>
+      <c r="H51" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="100">
+        <v>2</v>
+      </c>
+      <c r="E52" s="100" t="s">
+        <v>276</v>
+      </c>
+      <c r="F52" s="100">
+        <v>1</v>
+      </c>
+      <c r="G52" s="102">
+        <v>45250</v>
+      </c>
+      <c r="H52" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D53" s="100">
+        <v>3</v>
+      </c>
+      <c r="E53" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="F53" s="100">
+        <v>2</v>
+      </c>
+      <c r="G53" s="102">
+        <v>45250</v>
+      </c>
+      <c r="H53" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D55" s="98" t="s">
+        <v>278</v>
+      </c>
+      <c r="E55" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="G55" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="I55" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="J55" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D56" s="100">
+        <v>1</v>
+      </c>
+      <c r="E56" s="100" t="s">
+        <v>280</v>
+      </c>
+      <c r="F56" s="100">
+        <v>5</v>
+      </c>
+      <c r="G56" s="105">
+        <v>1</v>
+      </c>
+      <c r="H56" s="105">
+        <v>1</v>
+      </c>
+      <c r="I56" s="102">
+        <v>45250</v>
+      </c>
+      <c r="J56" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D57" s="100">
+        <v>2</v>
+      </c>
+      <c r="E57" s="100" t="s">
+        <v>281</v>
+      </c>
+      <c r="F57" s="100">
+        <v>0</v>
+      </c>
+      <c r="G57" s="105">
+        <v>2</v>
+      </c>
+      <c r="H57" s="105">
+        <v>2</v>
+      </c>
+      <c r="I57" s="102">
+        <v>45250</v>
+      </c>
+      <c r="J57" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D59" s="98" t="s">
+        <v>282</v>
+      </c>
+      <c r="E59" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="F59" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="G59" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="H59" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="I59" s="103" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D60" s="100">
+        <v>1</v>
+      </c>
+      <c r="E60" s="100">
+        <v>1</v>
+      </c>
+      <c r="F60" s="100">
+        <v>1</v>
+      </c>
+      <c r="G60" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="H60" s="102">
+        <v>45250</v>
+      </c>
+      <c r="I60" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D61" s="100">
+        <v>2</v>
+      </c>
+      <c r="E61" s="100">
+        <v>2</v>
+      </c>
+      <c r="F61" s="100">
+        <v>2</v>
+      </c>
+      <c r="G61" s="100" t="s">
+        <v>284</v>
+      </c>
+      <c r="H61" s="102">
+        <v>45250</v>
+      </c>
+      <c r="I61" s="102">
+        <v>45250</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{A873153E-40DB-41B6-8E2F-C71DC55AA566}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{206963B5-E983-4E50-8EF5-13FD7186C55D}"/>
+    <hyperlink ref="G16" r:id="rId3" xr:uid="{507B468B-04D3-4F87-85A1-5F47153D1EAE}"/>
+    <hyperlink ref="G17" r:id="rId4" xr:uid="{FA57DAA9-A7C8-43B0-81BA-1F2C49F02DDC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FE1267-6E16-41A9-BAAC-A7D93E9BE927}">
   <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,7 +5391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C845AE0-CB31-46F0-8234-FCDAE7B695FB}">
   <dimension ref="B1:I34"/>
   <sheetViews>
@@ -4317,7 +5664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E76D66F-CD0A-4A14-A1CE-B0B9ADF79C35}">
   <dimension ref="B1:K76"/>
   <sheetViews>
@@ -5207,12 +6554,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48850B9-88D1-43C5-89E8-8935C18AB769}">
   <dimension ref="B1:P37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5608,16 +6955,16 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="110" t="s">
+      <c r="G27" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
-      <c r="N27" s="112"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="88"/>
       <c r="O27" s="9"/>
       <c r="P27" t="s">
         <v>43</v>
@@ -5628,14 +6975,14 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="113"/>
-      <c r="H28" s="114"/>
-      <c r="I28" s="114"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="113"/>
-      <c r="L28" s="114"/>
-      <c r="M28" s="114"/>
-      <c r="N28" s="115"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="91"/>
       <c r="O28" s="9"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
@@ -5643,14 +6990,14 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="117"/>
-      <c r="I29" s="117"/>
-      <c r="J29" s="118"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="117"/>
-      <c r="M29" s="117"/>
-      <c r="N29" s="118"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="94"/>
       <c r="O29" s="9"/>
     </row>
     <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5658,14 +7005,14 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="120"/>
-      <c r="I30" s="120"/>
-      <c r="J30" s="121"/>
-      <c r="K30" s="119"/>
-      <c r="L30" s="120"/>
-      <c r="M30" s="120"/>
-      <c r="N30" s="121"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="97"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="96"/>
+      <c r="N30" s="97"/>
       <c r="O30" s="9"/>
     </row>
     <row r="31" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5786,7 +7133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD2B5F3-EF1E-4B3E-A14A-654D765FCDEB}">
   <dimension ref="B1:M39"/>
   <sheetViews>
@@ -6321,7 +7668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F7FC25-C587-492D-843E-4772CE361F41}">
   <dimension ref="B1:K33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding user table with MySQL database
</commit_message>
<xml_diff>
--- a/Ecommerce.xlsx
+++ b/Ecommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\Proyectos_Personales\Ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0415AA1D-FF96-443B-9692-91451024A5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBBF8D6-E758-43E3-84C9-8C023AF7CB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{EC1BCCFC-3DC3-41C4-92E1-54DD98A85853}"/>
   </bookViews>
@@ -1572,11 +1572,96 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1606,81 +1691,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1719,16 +1729,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2109,16 +2109,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
@@ -2178,107 +2178,112 @@
     </row>
     <row r="11" spans="2:5" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="50"/>
+      <c r="C20" s="57"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="57"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="50"/>
+      <c r="C22" s="57"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="50"/>
+      <c r="C23" s="57"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="58"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B3:C3"/>
@@ -2292,11 +2297,6 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2322,22 +2322,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="35"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="24">
         <v>1</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C5" s="25" t="s">
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="81" t="s">
         <v>131</v>
       </c>
       <c r="D15" s="44" t="s">
@@ -2433,12 +2433,12 @@
       <c r="F15" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="84" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="62"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="43" t="s">
         <v>74</v>
       </c>
@@ -2446,10 +2446,10 @@
         <v>115</v>
       </c>
       <c r="F16" s="46"/>
-      <c r="G16" s="52"/>
+      <c r="G16" s="85"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="62"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="43" t="s">
         <v>75</v>
       </c>
@@ -2457,10 +2457,10 @@
         <v>115</v>
       </c>
       <c r="F17" s="46"/>
-      <c r="G17" s="52"/>
+      <c r="G17" s="85"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="62"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="43" t="s">
         <v>73</v>
       </c>
@@ -2470,10 +2470,10 @@
       <c r="F18" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="85"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="62"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="43" t="s">
         <v>76</v>
       </c>
@@ -2481,10 +2481,10 @@
         <v>117</v>
       </c>
       <c r="F19" s="46"/>
-      <c r="G19" s="52"/>
+      <c r="G19" s="85"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="62"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="43" t="s">
         <v>118</v>
       </c>
@@ -2494,10 +2494,10 @@
       <c r="F20" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G20" s="52"/>
+      <c r="G20" s="85"/>
     </row>
     <row r="21" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="63"/>
+      <c r="C21" s="83"/>
       <c r="D21" s="47" t="s">
         <v>77</v>
       </c>
@@ -2505,10 +2505,10 @@
         <v>117</v>
       </c>
       <c r="F21" s="48"/>
-      <c r="G21" s="53"/>
+      <c r="G21" s="86"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="81" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -2520,10 +2520,10 @@
       <c r="F22" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="87"/>
     </row>
     <row r="23" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="62"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="43" t="s">
         <v>78</v>
       </c>
@@ -2531,10 +2531,10 @@
         <v>121</v>
       </c>
       <c r="F23" s="46"/>
-      <c r="G23" s="55"/>
+      <c r="G23" s="88"/>
     </row>
     <row r="24" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="63"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="47" t="s">
         <v>79</v>
       </c>
@@ -2542,10 +2542,10 @@
         <v>121</v>
       </c>
       <c r="F24" s="48"/>
-      <c r="G24" s="56"/>
+      <c r="G24" s="89"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="81" t="s">
         <v>80</v>
       </c>
       <c r="D25" s="44" t="s">
@@ -2557,12 +2557,12 @@
       <c r="F25" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="90" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="62"/>
+      <c r="C26" s="82"/>
       <c r="D26" s="43" t="s">
         <v>81</v>
       </c>
@@ -2570,10 +2570,10 @@
         <v>116</v>
       </c>
       <c r="F26" s="46"/>
-      <c r="G26" s="58"/>
+      <c r="G26" s="91"/>
     </row>
     <row r="27" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="62"/>
+      <c r="C27" s="82"/>
       <c r="D27" s="43" t="s">
         <v>82</v>
       </c>
@@ -2581,10 +2581,10 @@
         <v>123</v>
       </c>
       <c r="F27" s="46"/>
-      <c r="G27" s="58"/>
+      <c r="G27" s="91"/>
     </row>
     <row r="28" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="62"/>
+      <c r="C28" s="82"/>
       <c r="D28" s="43" t="s">
         <v>101</v>
       </c>
@@ -2594,10 +2594,10 @@
       <c r="F28" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="58"/>
+      <c r="G28" s="91"/>
     </row>
     <row r="29" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="62"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="43" t="s">
         <v>103</v>
       </c>
@@ -2607,10 +2607,10 @@
       <c r="F29" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="58"/>
+      <c r="G29" s="91"/>
     </row>
     <row r="30" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="62"/>
+      <c r="C30" s="82"/>
       <c r="D30" s="43" t="s">
         <v>129</v>
       </c>
@@ -2620,10 +2620,10 @@
       <c r="F30" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="58"/>
+      <c r="G30" s="91"/>
     </row>
     <row r="31" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="62"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="43" t="s">
         <v>122</v>
       </c>
@@ -2633,10 +2633,10 @@
       <c r="F31" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="58"/>
+      <c r="G31" s="91"/>
     </row>
     <row r="32" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="62"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="43" t="s">
         <v>113</v>
       </c>
@@ -2646,10 +2646,10 @@
       <c r="F32" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="58"/>
+      <c r="G32" s="91"/>
     </row>
     <row r="33" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="62"/>
+      <c r="C33" s="82"/>
       <c r="D33" s="43" t="s">
         <v>85</v>
       </c>
@@ -2657,10 +2657,10 @@
         <v>114</v>
       </c>
       <c r="F33" s="46"/>
-      <c r="G33" s="58"/>
+      <c r="G33" s="91"/>
     </row>
     <row r="34" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="62"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="43" t="s">
         <v>91</v>
       </c>
@@ -2670,10 +2670,10 @@
       <c r="F34" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="58"/>
+      <c r="G34" s="91"/>
     </row>
     <row r="35" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="62"/>
+      <c r="C35" s="82"/>
       <c r="D35" s="43" t="s">
         <v>79</v>
       </c>
@@ -2681,10 +2681,10 @@
         <v>121</v>
       </c>
       <c r="F35" s="46"/>
-      <c r="G35" s="58"/>
+      <c r="G35" s="91"/>
     </row>
     <row r="36" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="63"/>
+      <c r="C36" s="83"/>
       <c r="D36" s="47" t="s">
         <v>86</v>
       </c>
@@ -2692,10 +2692,10 @@
         <v>121</v>
       </c>
       <c r="F36" s="48"/>
-      <c r="G36" s="59"/>
+      <c r="G36" s="92"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="76" t="s">
         <v>109</v>
       </c>
       <c r="D37" s="44" t="s">
@@ -2707,10 +2707,10 @@
       <c r="F37" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G37" s="54"/>
+      <c r="G37" s="87"/>
     </row>
     <row r="38" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="68"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="43" t="s">
         <v>89</v>
       </c>
@@ -2720,10 +2720,10 @@
       <c r="F38" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G38" s="55"/>
+      <c r="G38" s="88"/>
     </row>
     <row r="39" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="68"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="43" t="s">
         <v>111</v>
       </c>
@@ -2731,10 +2731,10 @@
         <v>121</v>
       </c>
       <c r="F39" s="46"/>
-      <c r="G39" s="55"/>
+      <c r="G39" s="88"/>
     </row>
     <row r="40" spans="3:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="69"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="47" t="s">
         <v>112</v>
       </c>
@@ -2742,10 +2742,10 @@
         <v>124</v>
       </c>
       <c r="F40" s="48"/>
-      <c r="G40" s="56"/>
+      <c r="G40" s="89"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="81" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="44" t="s">
@@ -2760,7 +2760,7 @@
       <c r="G41" s="45"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="62"/>
+      <c r="C42" s="82"/>
       <c r="D42" s="43" t="s">
         <v>87</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="G42" s="46"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="62"/>
+      <c r="C43" s="82"/>
       <c r="D43" s="43" t="s">
         <v>125</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="G43" s="46"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="62"/>
+      <c r="C44" s="82"/>
       <c r="D44" s="43" t="s">
         <v>78</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="G44" s="46"/>
     </row>
     <row r="45" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="63"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="47" t="s">
         <v>79</v>
       </c>
@@ -2806,7 +2806,7 @@
       <c r="G45" s="48"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="81" t="s">
         <v>88</v>
       </c>
       <c r="D46" s="44" t="s">
@@ -2821,7 +2821,7 @@
       <c r="G46" s="45"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="62"/>
+      <c r="C47" s="82"/>
       <c r="D47" s="43" t="s">
         <v>89</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="G47" s="46"/>
     </row>
     <row r="48" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="63"/>
+      <c r="C48" s="83"/>
       <c r="D48" s="47" t="s">
         <v>90</v>
       </c>
@@ -2845,7 +2845,7 @@
       <c r="G48" s="48"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C49" s="61" t="s">
+      <c r="C49" s="81" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="44" t="s">
@@ -2860,7 +2860,7 @@
       <c r="G49" s="45"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C50" s="62"/>
+      <c r="C50" s="82"/>
       <c r="D50" s="43" t="s">
         <v>90</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="G50" s="46"/>
     </row>
     <row r="51" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="63"/>
+      <c r="C51" s="83"/>
       <c r="D51" s="47" t="s">
         <v>94</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="G51" s="48"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="81" t="s">
         <v>201</v>
       </c>
       <c r="D52" s="44" t="s">
@@ -2897,7 +2897,7 @@
       <c r="G52" s="45"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C53" s="62"/>
+      <c r="C53" s="82"/>
       <c r="D53" s="43" t="s">
         <v>87</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="G53" s="46"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C54" s="62"/>
+      <c r="C54" s="82"/>
       <c r="D54" s="43" t="s">
         <v>85</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="G54" s="46"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C55" s="62"/>
+      <c r="C55" s="82"/>
       <c r="D55" s="43" t="s">
         <v>172</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="G55" s="46"/>
     </row>
     <row r="56" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="63"/>
+      <c r="C56" s="83"/>
       <c r="D56" s="47" t="s">
         <v>214</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="I60" s="28"/>
     </row>
     <row r="61" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C61" s="70" t="s">
+      <c r="C61" s="79" t="s">
         <v>120</v>
       </c>
       <c r="D61" s="43" t="s">
@@ -2989,7 +2989,7 @@
       <c r="H61" s="28"/>
     </row>
     <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C62" s="71"/>
+      <c r="C62" s="80"/>
       <c r="D62" s="43" t="s">
         <v>119</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="G62" s="39"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="75" t="s">
         <v>84</v>
       </c>
       <c r="D63" s="43" t="s">
@@ -3017,7 +3017,7 @@
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C64" s="64"/>
+      <c r="C64" s="75"/>
       <c r="D64" s="43" t="s">
         <v>84</v>
       </c>
@@ -3028,7 +3028,7 @@
       <c r="H64" s="28"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C65" s="64" t="s">
+      <c r="C65" s="75" t="s">
         <v>102</v>
       </c>
       <c r="D65" s="43" t="s">
@@ -3045,7 +3045,7 @@
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C66" s="64"/>
+      <c r="C66" s="75"/>
       <c r="D66" s="43" t="s">
         <v>83</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="H66" s="28"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C67" s="65" t="s">
+      <c r="C67" s="72" t="s">
         <v>104</v>
       </c>
       <c r="D67" s="43" t="s">
@@ -3074,7 +3074,7 @@
       <c r="I67" s="28"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C68" s="66"/>
+      <c r="C68" s="73"/>
       <c r="D68" s="43" t="s">
         <v>105</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C69" s="65" t="s">
+      <c r="C69" s="72" t="s">
         <v>54</v>
       </c>
       <c r="D69" s="43" t="s">
@@ -3098,7 +3098,7 @@
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C70" s="66"/>
+      <c r="C70" s="73"/>
       <c r="D70" s="43" t="s">
         <v>108</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="65" t="s">
+      <c r="C71" s="72" t="s">
         <v>171</v>
       </c>
       <c r="D71" s="43" t="s">
@@ -3125,7 +3125,7 @@
       </c>
     </row>
     <row r="72" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="C72" s="66"/>
+      <c r="C72" s="73"/>
       <c r="D72" s="43" t="s">
         <v>171</v>
       </c>
@@ -3150,694 +3150,752 @@
       <c r="D76" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="E76" s="84" t="s">
+      <c r="E76" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="F76" s="84"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="84"/>
-      <c r="I76" s="84"/>
-      <c r="J76" s="84"/>
-      <c r="K76" s="84"/>
+      <c r="F76" s="63"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="63"/>
+      <c r="J76" s="63"/>
+      <c r="K76" s="63"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C77" s="78" t="s">
+      <c r="C77" s="69" t="s">
         <v>131</v>
       </c>
       <c r="D77" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="E77" s="76"/>
-      <c r="F77" s="76"/>
-      <c r="G77" s="76"/>
-      <c r="H77" s="76"/>
-      <c r="I77" s="76"/>
-      <c r="J77" s="76"/>
-      <c r="K77" s="77"/>
+      <c r="E77" s="65"/>
+      <c r="F77" s="65"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="65"/>
+      <c r="J77" s="65"/>
+      <c r="K77" s="66"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C78" s="79"/>
+      <c r="C78" s="70"/>
       <c r="D78" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="72" t="s">
+      <c r="E78" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="F78" s="72"/>
-      <c r="G78" s="72"/>
-      <c r="H78" s="72"/>
-      <c r="I78" s="72"/>
-      <c r="J78" s="72"/>
-      <c r="K78" s="73"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="59"/>
+      <c r="K78" s="60"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C79" s="79"/>
+      <c r="C79" s="70"/>
       <c r="D79" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="E79" s="72" t="s">
+      <c r="E79" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="F79" s="72"/>
-      <c r="G79" s="72"/>
-      <c r="H79" s="72"/>
-      <c r="I79" s="72"/>
-      <c r="J79" s="72"/>
-      <c r="K79" s="73"/>
+      <c r="F79" s="59"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="59"/>
+      <c r="J79" s="59"/>
+      <c r="K79" s="60"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C80" s="79"/>
+      <c r="C80" s="70"/>
       <c r="D80" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="72" t="s">
+      <c r="E80" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="F80" s="72"/>
-      <c r="G80" s="72"/>
-      <c r="H80" s="72"/>
-      <c r="I80" s="72"/>
-      <c r="J80" s="72"/>
-      <c r="K80" s="73"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="59"/>
+      <c r="H80" s="59"/>
+      <c r="I80" s="59"/>
+      <c r="J80" s="59"/>
+      <c r="K80" s="60"/>
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C81" s="81"/>
+      <c r="C81" s="74"/>
       <c r="D81" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="72"/>
-      <c r="G81" s="72"/>
-      <c r="H81" s="72"/>
-      <c r="I81" s="72"/>
-      <c r="J81" s="72"/>
-      <c r="K81" s="73"/>
+      <c r="E81" s="59"/>
+      <c r="F81" s="59"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="59"/>
+      <c r="J81" s="59"/>
+      <c r="K81" s="60"/>
     </row>
     <row r="82" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="80"/>
+      <c r="C82" s="71"/>
       <c r="D82" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="E82" s="74" t="s">
+      <c r="E82" s="61" t="s">
         <v>189</v>
       </c>
-      <c r="F82" s="74"/>
-      <c r="G82" s="74"/>
-      <c r="H82" s="74"/>
-      <c r="I82" s="74"/>
-      <c r="J82" s="74"/>
-      <c r="K82" s="75"/>
+      <c r="F82" s="61"/>
+      <c r="G82" s="61"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="61"/>
+      <c r="K82" s="62"/>
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C83" s="78" t="s">
+      <c r="C83" s="69" t="s">
         <v>61</v>
       </c>
       <c r="D83" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E83" s="76" t="s">
+      <c r="E83" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="F83" s="76"/>
-      <c r="G83" s="76"/>
-      <c r="H83" s="76"/>
-      <c r="I83" s="76"/>
-      <c r="J83" s="76"/>
-      <c r="K83" s="77"/>
+      <c r="F83" s="65"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="66"/>
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C84" s="79"/>
+      <c r="C84" s="70"/>
       <c r="D84" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="E84" s="72" t="s">
+      <c r="E84" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="F84" s="72"/>
-      <c r="G84" s="72"/>
-      <c r="H84" s="72"/>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="73"/>
+      <c r="F84" s="59"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="59"/>
+      <c r="I84" s="59"/>
+      <c r="J84" s="59"/>
+      <c r="K84" s="60"/>
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C85" s="79"/>
+      <c r="C85" s="70"/>
       <c r="D85" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="E85" s="72" t="s">
+      <c r="E85" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="F85" s="72"/>
-      <c r="G85" s="72"/>
-      <c r="H85" s="72"/>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="73"/>
+      <c r="F85" s="59"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="59"/>
+      <c r="J85" s="59"/>
+      <c r="K85" s="60"/>
     </row>
     <row r="86" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="80"/>
+      <c r="C86" s="71"/>
       <c r="D86" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="E86" s="74" t="s">
+      <c r="E86" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="74"/>
-      <c r="I86" s="74"/>
-      <c r="J86" s="74"/>
-      <c r="K86" s="75"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="61"/>
+      <c r="I86" s="61"/>
+      <c r="J86" s="61"/>
+      <c r="K86" s="62"/>
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C87" s="78" t="s">
+      <c r="C87" s="69" t="s">
         <v>80</v>
       </c>
       <c r="D87" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="E87" s="76" t="s">
+      <c r="E87" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="F87" s="76"/>
-      <c r="G87" s="76"/>
-      <c r="H87" s="76"/>
-      <c r="I87" s="76"/>
-      <c r="J87" s="76"/>
-      <c r="K87" s="77"/>
+      <c r="F87" s="65"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="66"/>
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C88" s="79"/>
+      <c r="C88" s="70"/>
       <c r="D88" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="E88" s="72"/>
-      <c r="F88" s="72"/>
-      <c r="G88" s="72"/>
-      <c r="H88" s="72"/>
-      <c r="I88" s="72"/>
-      <c r="J88" s="72"/>
-      <c r="K88" s="73"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
+      <c r="G88" s="59"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="59"/>
+      <c r="J88" s="59"/>
+      <c r="K88" s="60"/>
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C89" s="79"/>
+      <c r="C89" s="70"/>
       <c r="D89" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="E89" s="72"/>
-      <c r="F89" s="72"/>
-      <c r="G89" s="72"/>
-      <c r="H89" s="72"/>
-      <c r="I89" s="72"/>
-      <c r="J89" s="72"/>
-      <c r="K89" s="73"/>
+      <c r="E89" s="59"/>
+      <c r="F89" s="59"/>
+      <c r="G89" s="59"/>
+      <c r="H89" s="59"/>
+      <c r="I89" s="59"/>
+      <c r="J89" s="59"/>
+      <c r="K89" s="60"/>
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C90" s="79"/>
+      <c r="C90" s="70"/>
       <c r="D90" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="E90" s="72" t="s">
+      <c r="E90" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="F90" s="72"/>
-      <c r="G90" s="72"/>
-      <c r="H90" s="72"/>
-      <c r="I90" s="72"/>
-      <c r="J90" s="72"/>
-      <c r="K90" s="73"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="59"/>
+      <c r="J90" s="59"/>
+      <c r="K90" s="60"/>
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C91" s="79"/>
+      <c r="C91" s="70"/>
       <c r="D91" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="72" t="s">
+      <c r="E91" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="F91" s="72"/>
-      <c r="G91" s="72"/>
-      <c r="H91" s="72"/>
-      <c r="I91" s="72"/>
-      <c r="J91" s="72"/>
-      <c r="K91" s="73"/>
+      <c r="F91" s="59"/>
+      <c r="G91" s="59"/>
+      <c r="H91" s="59"/>
+      <c r="I91" s="59"/>
+      <c r="J91" s="59"/>
+      <c r="K91" s="60"/>
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C92" s="79"/>
+      <c r="C92" s="70"/>
       <c r="D92" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="E92" s="72" t="s">
+      <c r="E92" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="F92" s="72"/>
-      <c r="G92" s="72"/>
-      <c r="H92" s="72"/>
-      <c r="I92" s="72"/>
-      <c r="J92" s="72"/>
-      <c r="K92" s="73"/>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="59"/>
+      <c r="J92" s="59"/>
+      <c r="K92" s="60"/>
     </row>
     <row r="93" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C93" s="79"/>
+      <c r="C93" s="70"/>
       <c r="D93" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="E93" s="72" t="s">
+      <c r="E93" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="F93" s="72"/>
-      <c r="G93" s="72"/>
-      <c r="H93" s="72"/>
-      <c r="I93" s="72"/>
-      <c r="J93" s="72"/>
-      <c r="K93" s="73"/>
+      <c r="F93" s="59"/>
+      <c r="G93" s="59"/>
+      <c r="H93" s="59"/>
+      <c r="I93" s="59"/>
+      <c r="J93" s="59"/>
+      <c r="K93" s="60"/>
     </row>
     <row r="94" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="81"/>
+      <c r="C94" s="74"/>
       <c r="D94" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="E94" s="82" t="s">
+      <c r="E94" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="F94" s="82"/>
-      <c r="G94" s="82"/>
-      <c r="H94" s="82"/>
-      <c r="I94" s="82"/>
-      <c r="J94" s="82"/>
-      <c r="K94" s="83"/>
+      <c r="F94" s="67"/>
+      <c r="G94" s="67"/>
+      <c r="H94" s="67"/>
+      <c r="I94" s="67"/>
+      <c r="J94" s="67"/>
+      <c r="K94" s="68"/>
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C95" s="78" t="s">
+      <c r="C95" s="69" t="s">
         <v>201</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="E95" s="76" t="s">
+      <c r="E95" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="F95" s="76"/>
-      <c r="G95" s="76"/>
-      <c r="H95" s="76"/>
-      <c r="I95" s="76"/>
-      <c r="J95" s="76"/>
-      <c r="K95" s="77"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="66"/>
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C96" s="79"/>
+      <c r="C96" s="70"/>
       <c r="D96" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="E96" s="72" t="s">
+      <c r="E96" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="F96" s="72"/>
-      <c r="G96" s="72"/>
-      <c r="H96" s="72"/>
-      <c r="I96" s="72"/>
-      <c r="J96" s="72"/>
-      <c r="K96" s="73"/>
+      <c r="F96" s="59"/>
+      <c r="G96" s="59"/>
+      <c r="H96" s="59"/>
+      <c r="I96" s="59"/>
+      <c r="J96" s="59"/>
+      <c r="K96" s="60"/>
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C97" s="79"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="F97" s="72"/>
-      <c r="G97" s="72"/>
-      <c r="H97" s="72"/>
-      <c r="I97" s="72"/>
-      <c r="J97" s="72"/>
-      <c r="K97" s="73"/>
+      <c r="F97" s="59"/>
+      <c r="G97" s="59"/>
+      <c r="H97" s="59"/>
+      <c r="I97" s="59"/>
+      <c r="J97" s="59"/>
+      <c r="K97" s="60"/>
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C98" s="79"/>
+      <c r="C98" s="70"/>
       <c r="D98" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="E98" s="72" t="s">
+      <c r="E98" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="F98" s="72"/>
-      <c r="G98" s="72"/>
-      <c r="H98" s="72"/>
-      <c r="I98" s="72"/>
-      <c r="J98" s="72"/>
-      <c r="K98" s="73"/>
+      <c r="F98" s="59"/>
+      <c r="G98" s="59"/>
+      <c r="H98" s="59"/>
+      <c r="I98" s="59"/>
+      <c r="J98" s="59"/>
+      <c r="K98" s="60"/>
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C99" s="79"/>
+      <c r="C99" s="70"/>
       <c r="D99" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="E99" s="72" t="s">
+      <c r="E99" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="F99" s="72"/>
-      <c r="G99" s="72"/>
-      <c r="H99" s="72"/>
-      <c r="I99" s="72"/>
-      <c r="J99" s="72"/>
-      <c r="K99" s="73"/>
+      <c r="F99" s="59"/>
+      <c r="G99" s="59"/>
+      <c r="H99" s="59"/>
+      <c r="I99" s="59"/>
+      <c r="J99" s="59"/>
+      <c r="K99" s="60"/>
     </row>
     <row r="100" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="80"/>
+      <c r="C100" s="71"/>
       <c r="D100" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="E100" s="74" t="s">
+      <c r="E100" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="F100" s="74"/>
-      <c r="G100" s="74"/>
-      <c r="H100" s="74"/>
-      <c r="I100" s="74"/>
-      <c r="J100" s="74"/>
-      <c r="K100" s="75"/>
+      <c r="F100" s="61"/>
+      <c r="G100" s="61"/>
+      <c r="H100" s="61"/>
+      <c r="I100" s="61"/>
+      <c r="J100" s="61"/>
+      <c r="K100" s="62"/>
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C101" s="78" t="s">
+      <c r="C101" s="69" t="s">
         <v>109</v>
       </c>
       <c r="D101" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="E101" s="76" t="s">
+      <c r="E101" s="65" t="s">
         <v>187</v>
       </c>
-      <c r="F101" s="76"/>
-      <c r="G101" s="76"/>
-      <c r="H101" s="76"/>
-      <c r="I101" s="76"/>
-      <c r="J101" s="76"/>
-      <c r="K101" s="77"/>
+      <c r="F101" s="65"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="65"/>
+      <c r="I101" s="65"/>
+      <c r="J101" s="65"/>
+      <c r="K101" s="66"/>
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C102" s="79"/>
+      <c r="C102" s="70"/>
       <c r="D102" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="E102" s="72"/>
-      <c r="F102" s="72"/>
-      <c r="G102" s="72"/>
-      <c r="H102" s="72"/>
-      <c r="I102" s="72"/>
-      <c r="J102" s="72"/>
-      <c r="K102" s="73"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="59"/>
+      <c r="G102" s="59"/>
+      <c r="H102" s="59"/>
+      <c r="I102" s="59"/>
+      <c r="J102" s="59"/>
+      <c r="K102" s="60"/>
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C103" s="79"/>
+      <c r="C103" s="70"/>
       <c r="D103" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="E103" s="72"/>
-      <c r="F103" s="72"/>
-      <c r="G103" s="72"/>
-      <c r="H103" s="72"/>
-      <c r="I103" s="72"/>
-      <c r="J103" s="72"/>
-      <c r="K103" s="73"/>
+      <c r="E103" s="59"/>
+      <c r="F103" s="59"/>
+      <c r="G103" s="59"/>
+      <c r="H103" s="59"/>
+      <c r="I103" s="59"/>
+      <c r="J103" s="59"/>
+      <c r="K103" s="60"/>
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C104" s="79"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="E104" s="72" t="s">
+      <c r="E104" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="F104" s="72"/>
-      <c r="G104" s="72"/>
-      <c r="H104" s="72"/>
-      <c r="I104" s="72"/>
-      <c r="J104" s="72"/>
-      <c r="K104" s="73"/>
+      <c r="F104" s="59"/>
+      <c r="G104" s="59"/>
+      <c r="H104" s="59"/>
+      <c r="I104" s="59"/>
+      <c r="J104" s="59"/>
+      <c r="K104" s="60"/>
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C105" s="79"/>
+      <c r="C105" s="70"/>
       <c r="D105" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E105" s="72" t="s">
+      <c r="E105" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="F105" s="72"/>
-      <c r="G105" s="72"/>
-      <c r="H105" s="72"/>
-      <c r="I105" s="72"/>
-      <c r="J105" s="72"/>
-      <c r="K105" s="73"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="59"/>
+      <c r="H105" s="59"/>
+      <c r="I105" s="59"/>
+      <c r="J105" s="59"/>
+      <c r="K105" s="60"/>
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C106" s="79"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="E106" s="72"/>
-      <c r="F106" s="72"/>
-      <c r="G106" s="72"/>
-      <c r="H106" s="72"/>
-      <c r="I106" s="72"/>
-      <c r="J106" s="72"/>
-      <c r="K106" s="73"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="59"/>
+      <c r="H106" s="59"/>
+      <c r="I106" s="59"/>
+      <c r="J106" s="59"/>
+      <c r="K106" s="60"/>
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C107" s="79"/>
+      <c r="C107" s="70"/>
       <c r="D107" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="E107" s="72" t="s">
+      <c r="E107" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="F107" s="72"/>
-      <c r="G107" s="72"/>
-      <c r="H107" s="72"/>
-      <c r="I107" s="72"/>
-      <c r="J107" s="72"/>
-      <c r="K107" s="73"/>
+      <c r="F107" s="59"/>
+      <c r="G107" s="59"/>
+      <c r="H107" s="59"/>
+      <c r="I107" s="59"/>
+      <c r="J107" s="59"/>
+      <c r="K107" s="60"/>
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C108" s="79"/>
+      <c r="C108" s="70"/>
       <c r="D108" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="E108" s="72" t="s">
+      <c r="E108" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="F108" s="72"/>
-      <c r="G108" s="72"/>
-      <c r="H108" s="72"/>
-      <c r="I108" s="72"/>
-      <c r="J108" s="72"/>
-      <c r="K108" s="73"/>
+      <c r="F108" s="59"/>
+      <c r="G108" s="59"/>
+      <c r="H108" s="59"/>
+      <c r="I108" s="59"/>
+      <c r="J108" s="59"/>
+      <c r="K108" s="60"/>
     </row>
     <row r="109" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C109" s="80"/>
+      <c r="C109" s="71"/>
       <c r="D109" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E109" s="74" t="s">
+      <c r="E109" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="F109" s="74"/>
-      <c r="G109" s="74"/>
-      <c r="H109" s="74"/>
-      <c r="I109" s="74"/>
-      <c r="J109" s="74"/>
-      <c r="K109" s="75"/>
+      <c r="F109" s="61"/>
+      <c r="G109" s="61"/>
+      <c r="H109" s="61"/>
+      <c r="I109" s="61"/>
+      <c r="J109" s="61"/>
+      <c r="K109" s="62"/>
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C110" s="78" t="s">
+      <c r="C110" s="69" t="s">
         <v>22</v>
       </c>
       <c r="D110" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="E110" s="76" t="s">
+      <c r="E110" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="F110" s="76"/>
-      <c r="G110" s="76"/>
-      <c r="H110" s="76"/>
-      <c r="I110" s="76"/>
-      <c r="J110" s="76"/>
-      <c r="K110" s="77"/>
+      <c r="F110" s="65"/>
+      <c r="G110" s="65"/>
+      <c r="H110" s="65"/>
+      <c r="I110" s="65"/>
+      <c r="J110" s="65"/>
+      <c r="K110" s="66"/>
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C111" s="79"/>
+      <c r="C111" s="70"/>
       <c r="D111" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="E111" s="72"/>
-      <c r="F111" s="72"/>
-      <c r="G111" s="72"/>
-      <c r="H111" s="72"/>
-      <c r="I111" s="72"/>
-      <c r="J111" s="72"/>
-      <c r="K111" s="73"/>
+      <c r="E111" s="59"/>
+      <c r="F111" s="59"/>
+      <c r="G111" s="59"/>
+      <c r="H111" s="59"/>
+      <c r="I111" s="59"/>
+      <c r="J111" s="59"/>
+      <c r="K111" s="60"/>
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C112" s="79"/>
+      <c r="C112" s="70"/>
       <c r="D112" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="E112" s="72" t="s">
+      <c r="E112" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="F112" s="72"/>
-      <c r="G112" s="72"/>
-      <c r="H112" s="72"/>
-      <c r="I112" s="72"/>
-      <c r="J112" s="72"/>
-      <c r="K112" s="73"/>
+      <c r="F112" s="59"/>
+      <c r="G112" s="59"/>
+      <c r="H112" s="59"/>
+      <c r="I112" s="59"/>
+      <c r="J112" s="59"/>
+      <c r="K112" s="60"/>
     </row>
     <row r="113" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="80"/>
+      <c r="C113" s="71"/>
       <c r="D113" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E113" s="74" t="s">
+      <c r="E113" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="F113" s="74"/>
-      <c r="G113" s="74"/>
-      <c r="H113" s="74"/>
-      <c r="I113" s="74"/>
-      <c r="J113" s="74"/>
-      <c r="K113" s="75"/>
+      <c r="F113" s="61"/>
+      <c r="G113" s="61"/>
+      <c r="H113" s="61"/>
+      <c r="I113" s="61"/>
+      <c r="J113" s="61"/>
+      <c r="K113" s="62"/>
     </row>
     <row r="114" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C114" s="78" t="s">
+      <c r="C114" s="69" t="s">
         <v>88</v>
       </c>
       <c r="D114" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="E114" s="76" t="s">
+      <c r="E114" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="F114" s="76"/>
-      <c r="G114" s="76"/>
-      <c r="H114" s="76"/>
-      <c r="I114" s="76"/>
-      <c r="J114" s="76"/>
-      <c r="K114" s="77"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="65"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65"/>
+      <c r="J114" s="65"/>
+      <c r="K114" s="66"/>
     </row>
     <row r="115" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C115" s="79"/>
+      <c r="C115" s="70"/>
       <c r="D115" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="E115" s="72" t="s">
+      <c r="E115" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="F115" s="72"/>
-      <c r="G115" s="72"/>
-      <c r="H115" s="72"/>
-      <c r="I115" s="72"/>
-      <c r="J115" s="72"/>
-      <c r="K115" s="73"/>
+      <c r="F115" s="59"/>
+      <c r="G115" s="59"/>
+      <c r="H115" s="59"/>
+      <c r="I115" s="59"/>
+      <c r="J115" s="59"/>
+      <c r="K115" s="60"/>
     </row>
     <row r="116" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C116" s="79"/>
+      <c r="C116" s="70"/>
       <c r="D116" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="E116" s="72" t="s">
+      <c r="E116" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="F116" s="72"/>
-      <c r="G116" s="72"/>
-      <c r="H116" s="72"/>
-      <c r="I116" s="72"/>
-      <c r="J116" s="72"/>
-      <c r="K116" s="73"/>
+      <c r="F116" s="59"/>
+      <c r="G116" s="59"/>
+      <c r="H116" s="59"/>
+      <c r="I116" s="59"/>
+      <c r="J116" s="59"/>
+      <c r="K116" s="60"/>
     </row>
     <row r="117" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="80"/>
+      <c r="C117" s="71"/>
       <c r="D117" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="E117" s="74" t="s">
+      <c r="E117" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="F117" s="74"/>
-      <c r="G117" s="74"/>
-      <c r="H117" s="74"/>
-      <c r="I117" s="74"/>
-      <c r="J117" s="74"/>
-      <c r="K117" s="75"/>
+      <c r="F117" s="61"/>
+      <c r="G117" s="61"/>
+      <c r="H117" s="61"/>
+      <c r="I117" s="61"/>
+      <c r="J117" s="61"/>
+      <c r="K117" s="62"/>
     </row>
     <row r="118" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C118" s="78" t="s">
+      <c r="C118" s="69" t="s">
         <v>68</v>
       </c>
       <c r="D118" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E118" s="76" t="s">
+      <c r="E118" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F118" s="76"/>
-      <c r="G118" s="76"/>
-      <c r="H118" s="76"/>
-      <c r="I118" s="76"/>
-      <c r="J118" s="76"/>
-      <c r="K118" s="77"/>
+      <c r="F118" s="65"/>
+      <c r="G118" s="65"/>
+      <c r="H118" s="65"/>
+      <c r="I118" s="65"/>
+      <c r="J118" s="65"/>
+      <c r="K118" s="66"/>
     </row>
     <row r="119" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C119" s="79"/>
+      <c r="C119" s="70"/>
       <c r="D119" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="E119" s="72"/>
-      <c r="F119" s="72"/>
-      <c r="G119" s="72"/>
-      <c r="H119" s="72"/>
-      <c r="I119" s="72"/>
-      <c r="J119" s="72"/>
-      <c r="K119" s="73"/>
+      <c r="E119" s="59"/>
+      <c r="F119" s="59"/>
+      <c r="G119" s="59"/>
+      <c r="H119" s="59"/>
+      <c r="I119" s="59"/>
+      <c r="J119" s="59"/>
+      <c r="K119" s="60"/>
     </row>
     <row r="120" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C120" s="79"/>
+      <c r="C120" s="70"/>
       <c r="D120" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E120" s="72" t="s">
+      <c r="E120" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="F120" s="72"/>
-      <c r="G120" s="72"/>
-      <c r="H120" s="72"/>
-      <c r="I120" s="72"/>
-      <c r="J120" s="72"/>
-      <c r="K120" s="73"/>
+      <c r="F120" s="59"/>
+      <c r="G120" s="59"/>
+      <c r="H120" s="59"/>
+      <c r="I120" s="59"/>
+      <c r="J120" s="59"/>
+      <c r="K120" s="60"/>
     </row>
     <row r="121" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C121" s="80"/>
+      <c r="C121" s="71"/>
       <c r="D121" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="E121" s="74" t="s">
+      <c r="E121" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="F121" s="74"/>
-      <c r="G121" s="74"/>
-      <c r="H121" s="74"/>
-      <c r="I121" s="74"/>
-      <c r="J121" s="74"/>
-      <c r="K121" s="75"/>
+      <c r="F121" s="61"/>
+      <c r="G121" s="61"/>
+      <c r="H121" s="61"/>
+      <c r="I121" s="61"/>
+      <c r="J121" s="61"/>
+      <c r="K121" s="62"/>
     </row>
     <row r="122" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C122" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="G15:G21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="G25:G36"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C25:C36"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C41:C45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="E96:K96"/>
+    <mergeCell ref="E97:K97"/>
+    <mergeCell ref="E98:K98"/>
+    <mergeCell ref="E99:K99"/>
+    <mergeCell ref="E117:K117"/>
+    <mergeCell ref="E116:K116"/>
+    <mergeCell ref="E110:K110"/>
+    <mergeCell ref="E111:K111"/>
+    <mergeCell ref="E101:K101"/>
+    <mergeCell ref="E102:K102"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C95:C100"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="C87:C94"/>
+    <mergeCell ref="C101:C109"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="E118:K118"/>
+    <mergeCell ref="E119:K119"/>
+    <mergeCell ref="E120:K120"/>
+    <mergeCell ref="E121:K121"/>
+    <mergeCell ref="E95:K95"/>
+    <mergeCell ref="E112:K112"/>
+    <mergeCell ref="E113:K113"/>
+    <mergeCell ref="E114:K114"/>
+    <mergeCell ref="E115:K115"/>
+    <mergeCell ref="E103:K103"/>
+    <mergeCell ref="E104:K104"/>
+    <mergeCell ref="E105:K105"/>
+    <mergeCell ref="E106:K106"/>
+    <mergeCell ref="E107:K107"/>
+    <mergeCell ref="E108:K108"/>
+    <mergeCell ref="E109:K109"/>
+    <mergeCell ref="E87:K87"/>
+    <mergeCell ref="E88:K88"/>
+    <mergeCell ref="E89:K89"/>
+    <mergeCell ref="E90:K90"/>
+    <mergeCell ref="E94:K94"/>
     <mergeCell ref="E81:K81"/>
     <mergeCell ref="E100:K100"/>
     <mergeCell ref="E76:K76"/>
@@ -3854,64 +3912,6 @@
     <mergeCell ref="E84:K84"/>
     <mergeCell ref="E85:K85"/>
     <mergeCell ref="E86:K86"/>
-    <mergeCell ref="E87:K87"/>
-    <mergeCell ref="E88:K88"/>
-    <mergeCell ref="E89:K89"/>
-    <mergeCell ref="E90:K90"/>
-    <mergeCell ref="E94:K94"/>
-    <mergeCell ref="E118:K118"/>
-    <mergeCell ref="E119:K119"/>
-    <mergeCell ref="E120:K120"/>
-    <mergeCell ref="E121:K121"/>
-    <mergeCell ref="E95:K95"/>
-    <mergeCell ref="E112:K112"/>
-    <mergeCell ref="E113:K113"/>
-    <mergeCell ref="E114:K114"/>
-    <mergeCell ref="E115:K115"/>
-    <mergeCell ref="E103:K103"/>
-    <mergeCell ref="E104:K104"/>
-    <mergeCell ref="E105:K105"/>
-    <mergeCell ref="E106:K106"/>
-    <mergeCell ref="E107:K107"/>
-    <mergeCell ref="E108:K108"/>
-    <mergeCell ref="E109:K109"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C95:C100"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="C87:C94"/>
-    <mergeCell ref="C101:C109"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="E96:K96"/>
-    <mergeCell ref="E97:K97"/>
-    <mergeCell ref="E98:K98"/>
-    <mergeCell ref="E99:K99"/>
-    <mergeCell ref="E117:K117"/>
-    <mergeCell ref="E116:K116"/>
-    <mergeCell ref="E110:K110"/>
-    <mergeCell ref="E111:K111"/>
-    <mergeCell ref="E101:K101"/>
-    <mergeCell ref="E102:K102"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C41:C45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="G15:G21"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="G25:G36"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C25:C36"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C15:C21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3922,1139 +3922,1140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59B929-1572-41F9-B1E2-00E5AACADABB}">
-  <dimension ref="A2:N61"/>
+  <dimension ref="B2:O61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="C2" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="103" t="s">
+      <c r="E2" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="F2" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="G2" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="H2" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="I2" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="J2" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="103" t="s">
+      <c r="K2" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="103" t="s">
+      <c r="L2" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="L2" s="103" t="s">
+      <c r="M2" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="100">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="C3" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="100">
+      <c r="E3" s="51">
         <v>1</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="F3" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="100" t="s">
+      <c r="G3" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="G3" s="101" t="s">
+      <c r="H3" s="52" t="s">
         <v>247</v>
       </c>
-      <c r="H3" s="100">
+      <c r="I3" s="51">
         <v>5555555</v>
       </c>
-      <c r="I3" s="100">
+      <c r="J3" s="51">
         <v>123456789</v>
       </c>
-      <c r="J3" s="100">
+      <c r="K3" s="51">
         <v>1</v>
       </c>
-      <c r="K3" s="102">
+      <c r="L3" s="53">
         <v>45250</v>
       </c>
-      <c r="L3" s="102">
+      <c r="M3" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="100">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="51">
         <v>2</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="C4" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="D4" s="100">
+      <c r="E4" s="51">
         <v>2</v>
       </c>
-      <c r="E4" s="100" t="s">
+      <c r="F4" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="F4" s="100" t="s">
+      <c r="G4" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="G4" s="101" t="s">
+      <c r="H4" s="52" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="100">
+      <c r="I4" s="51">
         <v>2222222</v>
       </c>
-      <c r="I4" s="100">
+      <c r="J4" s="51">
         <v>123456789</v>
       </c>
-      <c r="J4" s="100">
+      <c r="K4" s="51">
         <v>2</v>
       </c>
-      <c r="K4" s="102">
+      <c r="L4" s="53">
         <v>45250</v>
       </c>
-      <c r="L4" s="102">
+      <c r="M4" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="C6" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="D6" s="98" t="s">
+      <c r="E6" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="F6" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="G6" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="98" t="s">
+      <c r="H6" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="98" t="s">
+      <c r="I6" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="J6" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="98" t="s">
+      <c r="K6" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="K6" s="98" t="s">
+      <c r="L6" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="L6" s="98" t="s">
+      <c r="M6" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="M6" s="103" t="s">
+      <c r="N6" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="N6" s="103" t="s">
+      <c r="O6" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="100">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="51">
         <v>1</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="C7" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="100">
+      <c r="E7" s="51">
         <v>1</v>
       </c>
-      <c r="E7" s="100" t="s">
+      <c r="F7" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="100">
+      <c r="G7" s="51">
         <v>100</v>
       </c>
-      <c r="G7" s="100">
+      <c r="H7" s="51">
         <v>20</v>
       </c>
-      <c r="H7" s="100" t="s">
+      <c r="I7" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="I7" s="100" t="s">
+      <c r="J7" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="J7" s="100">
+      <c r="K7" s="51">
         <v>0</v>
       </c>
-      <c r="K7" s="100">
+      <c r="L7" s="51">
         <v>0</v>
       </c>
-      <c r="L7" s="100">
+      <c r="M7" s="51">
         <v>5</v>
       </c>
-      <c r="M7" s="102">
+      <c r="N7" s="53">
         <v>45250</v>
       </c>
-      <c r="N7" s="102">
+      <c r="O7" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="100">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="51">
         <v>2</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="C8" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="D8" s="100">
+      <c r="E8" s="51">
         <v>2</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="F8" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="100">
+      <c r="G8" s="51">
         <v>110</v>
       </c>
-      <c r="G8" s="100">
+      <c r="H8" s="51">
         <v>15</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="I8" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="J8" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="J8" s="100">
+      <c r="K8" s="51">
         <v>0</v>
       </c>
-      <c r="K8" s="100">
+      <c r="L8" s="51">
         <v>0</v>
       </c>
-      <c r="L8" s="100">
+      <c r="M8" s="51">
         <v>5</v>
       </c>
-      <c r="M8" s="102">
+      <c r="N8" s="53">
         <v>45250</v>
       </c>
-      <c r="N8" s="102">
+      <c r="O8" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="51">
         <v>3</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="C9" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="100">
+      <c r="E9" s="51">
         <v>3</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="F9" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="100">
+      <c r="G9" s="51">
         <v>80</v>
       </c>
-      <c r="G9" s="100">
+      <c r="H9" s="51">
         <v>20</v>
       </c>
-      <c r="H9" s="100" t="s">
+      <c r="I9" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="I9" s="100" t="s">
+      <c r="J9" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="J9" s="100">
+      <c r="K9" s="51">
         <v>0</v>
       </c>
-      <c r="K9" s="100">
+      <c r="L9" s="51">
         <v>0</v>
       </c>
-      <c r="L9" s="100">
+      <c r="M9" s="51">
         <v>5</v>
       </c>
-      <c r="M9" s="102">
+      <c r="N9" s="53">
         <v>45250</v>
       </c>
-      <c r="N9" s="102">
+      <c r="O9" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="99" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="C11" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="E11" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="E11" s="103" t="s">
+      <c r="F11" s="54" t="s">
         <v>258</v>
       </c>
-      <c r="F11" s="103" t="s">
+      <c r="G11" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="G11" s="103" t="s">
+      <c r="H11" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="H11" s="103" t="s">
+      <c r="I11" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="I11" s="103" t="s">
+      <c r="J11" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="J11" s="103" t="s">
+      <c r="K11" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="K11" s="103" t="s">
+      <c r="L11" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="100">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="51">
         <v>1</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="C12" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="D12" s="100">
+      <c r="E12" s="51">
         <v>1</v>
       </c>
-      <c r="E12" s="100">
+      <c r="F12" s="51">
         <v>2</v>
       </c>
-      <c r="F12" s="100">
+      <c r="G12" s="51">
         <v>200</v>
       </c>
-      <c r="G12" s="100">
+      <c r="H12" s="51">
         <v>1</v>
       </c>
-      <c r="H12" s="100">
+      <c r="I12" s="51">
         <v>1</v>
       </c>
-      <c r="I12" s="100">
+      <c r="J12" s="51">
         <v>1</v>
       </c>
-      <c r="J12" s="102">
+      <c r="K12" s="53">
         <v>45250</v>
       </c>
-      <c r="K12" s="102">
+      <c r="L12" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="100">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="51">
         <v>2</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="C13" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="D13" s="100">
+      <c r="E13" s="51">
         <v>2</v>
       </c>
-      <c r="E13" s="100">
+      <c r="F13" s="51">
         <v>1</v>
       </c>
-      <c r="F13" s="100">
+      <c r="G13" s="51">
         <v>100</v>
       </c>
-      <c r="G13" s="100">
+      <c r="H13" s="51">
         <v>1</v>
       </c>
-      <c r="H13" s="100">
+      <c r="I13" s="51">
         <v>2</v>
       </c>
-      <c r="I13" s="100">
+      <c r="J13" s="51">
         <v>2</v>
       </c>
-      <c r="J13" s="102">
+      <c r="K13" s="53">
         <v>45250</v>
       </c>
-      <c r="K13" s="102">
+      <c r="L13" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="100">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="51">
         <v>3</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="C14" s="51" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="100">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="51">
         <v>4</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="C15" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="D15" s="103" t="s">
+      <c r="E15" s="54" t="s">
         <v>260</v>
       </c>
-      <c r="E15" s="103" t="s">
+      <c r="F15" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="103" t="s">
+      <c r="G15" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="103" t="s">
+      <c r="H15" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="103" t="s">
+      <c r="I15" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="103" t="s">
+      <c r="J15" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="103" t="s">
+      <c r="K15" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="103" t="s">
+      <c r="L15" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="L15" s="103" t="s">
+      <c r="M15" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="100">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="51">
         <v>1</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="F16" s="51" t="s">
         <v>245</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="G16" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="G16" s="101" t="s">
+      <c r="H16" s="52" t="s">
         <v>264</v>
       </c>
-      <c r="H16" s="100">
+      <c r="I16" s="51">
         <v>4444444</v>
       </c>
-      <c r="I16" s="100" t="s">
+      <c r="J16" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="J16" s="100" t="s">
+      <c r="K16" s="51" t="s">
         <v>268</v>
       </c>
-      <c r="K16" s="102">
+      <c r="L16" s="53">
         <v>45250</v>
       </c>
-      <c r="L16" s="102">
+      <c r="M16" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="99" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="C17" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="D17" s="100">
+      <c r="E17" s="51">
         <v>2</v>
       </c>
-      <c r="E17" s="100" t="s">
+      <c r="F17" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="F17" s="100" t="s">
+      <c r="G17" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="G17" s="101" t="s">
+      <c r="H17" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="H17" s="100">
+      <c r="I17" s="51">
         <v>777777</v>
       </c>
-      <c r="I17" s="100" t="s">
+      <c r="J17" s="51" t="s">
         <v>267</v>
       </c>
-      <c r="J17" s="100" t="s">
+      <c r="K17" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="K17" s="102">
+      <c r="L17" s="53">
         <v>45250</v>
       </c>
-      <c r="L17" s="102">
+      <c r="M17" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="100">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="51">
         <v>1</v>
       </c>
-      <c r="B18" s="100">
+      <c r="C18" s="51">
         <v>35</v>
       </c>
-      <c r="G18" s="104"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="100">
+      <c r="H18" s="55"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="100">
+      <c r="C19" s="51">
         <v>36</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="E19" s="49" t="s">
         <v>270</v>
       </c>
-      <c r="E19" s="98" t="s">
+      <c r="F19" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="G19" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="100">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="51">
         <v>3</v>
       </c>
-      <c r="B20" s="100">
+      <c r="C20" s="51">
         <v>37</v>
       </c>
-      <c r="D20" s="100">
+      <c r="E20" s="51">
         <v>1</v>
       </c>
-      <c r="E20" s="100">
+      <c r="F20" s="51">
         <v>1</v>
       </c>
-      <c r="F20" s="100">
+      <c r="G20" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="100">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="51">
         <v>4</v>
       </c>
-      <c r="B21" s="100">
+      <c r="C21" s="51">
         <v>38</v>
       </c>
-      <c r="D21" s="100">
+      <c r="E21" s="51">
         <v>2</v>
       </c>
-      <c r="E21" s="100">
+      <c r="F21" s="51">
         <v>2</v>
       </c>
-      <c r="F21" s="100">
+      <c r="G21" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="100">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="51">
         <v>5</v>
       </c>
-      <c r="B22" s="100">
+      <c r="C22" s="51">
         <v>39</v>
       </c>
-      <c r="D22" s="100">
+      <c r="E22" s="51">
         <v>3</v>
       </c>
-      <c r="E22" s="100">
+      <c r="F22" s="51">
         <v>3</v>
       </c>
-      <c r="F22" s="100">
+      <c r="G22" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="100">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="51">
         <v>6</v>
       </c>
-      <c r="B23" s="100">
+      <c r="C23" s="51">
         <v>40</v>
       </c>
-      <c r="D23" s="100">
+      <c r="E23" s="51">
         <v>4</v>
       </c>
-      <c r="E23" s="100">
+      <c r="F23" s="51">
         <v>4</v>
       </c>
-      <c r="F23" s="100">
+      <c r="G23" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="100">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="51">
         <v>7</v>
       </c>
-      <c r="B24" s="100">
+      <c r="C24" s="51">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="100">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="51">
         <v>8</v>
       </c>
-      <c r="B25" s="100">
+      <c r="C25" s="51">
         <v>42</v>
       </c>
-      <c r="D25" s="98" t="s">
+      <c r="E25" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="E25" s="98" t="s">
+      <c r="F25" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="F25" s="98" t="s">
+      <c r="G25" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="100">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="51">
         <v>1</v>
       </c>
-      <c r="E26" s="100">
+      <c r="F26" s="51">
         <v>1</v>
       </c>
-      <c r="F26" s="100">
+      <c r="G26" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="99" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="C27" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="D27" s="100">
+      <c r="E27" s="51">
         <v>2</v>
       </c>
-      <c r="E27" s="100">
+      <c r="F27" s="51">
         <v>2</v>
       </c>
-      <c r="F27" s="100">
+      <c r="G27" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="100">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="51">
         <v>1</v>
       </c>
-      <c r="B28" s="100" t="s">
+      <c r="C28" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="D28" s="100">
+      <c r="E28" s="51">
         <v>3</v>
       </c>
-      <c r="E28" s="100">
+      <c r="F28" s="51">
         <v>3</v>
       </c>
-      <c r="F28" s="100">
+      <c r="G28" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="100">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="51">
         <v>2</v>
       </c>
-      <c r="B29" s="100" t="s">
+      <c r="C29" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="D29" s="100">
+      <c r="E29" s="51">
         <v>4</v>
       </c>
-      <c r="E29" s="100">
+      <c r="F29" s="51">
         <v>6</v>
       </c>
-      <c r="F29" s="100">
+      <c r="G29" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="100">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="51">
         <v>3</v>
       </c>
-      <c r="B30" s="100" t="s">
+      <c r="C30" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="D30" s="100">
+      <c r="E30" s="51">
         <v>5</v>
       </c>
-      <c r="E30" s="100">
+      <c r="F30" s="51">
         <v>8</v>
       </c>
-      <c r="F30" s="100">
+      <c r="G30" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="100">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="51">
         <v>4</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="C31" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="D31" s="100">
+      <c r="E31" s="51">
         <v>6</v>
       </c>
-      <c r="E31" s="100">
+      <c r="F31" s="51">
         <v>2</v>
       </c>
-      <c r="F31" s="100">
+      <c r="G31" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="100">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="51">
         <v>5</v>
       </c>
-      <c r="B32" s="100" t="s">
+      <c r="C32" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="D32" s="100">
+      <c r="E32" s="51">
         <v>7</v>
       </c>
-      <c r="E32" s="100">
+      <c r="F32" s="51">
         <v>3</v>
       </c>
-      <c r="F32" s="100">
+      <c r="G32" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="100">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="51">
         <v>6</v>
       </c>
-      <c r="B33" s="100" t="s">
+      <c r="C33" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="D33" s="100">
+      <c r="E33" s="51">
         <v>8</v>
       </c>
-      <c r="E33" s="100">
+      <c r="F33" s="51">
         <v>7</v>
       </c>
-      <c r="F33" s="100">
+      <c r="G33" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="100">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="51">
         <v>7</v>
       </c>
-      <c r="B34" s="100" t="s">
+      <c r="C34" s="51" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="98" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="49" t="s">
         <v>272</v>
       </c>
-      <c r="E35" s="98" t="s">
+      <c r="F35" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="98" t="s">
+      <c r="G35" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="99" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="99" t="s">
+      <c r="C36" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="D36" s="100">
+      <c r="E36" s="51">
         <v>1</v>
       </c>
-      <c r="E36" s="100">
+      <c r="F36" s="51">
         <v>1</v>
       </c>
-      <c r="F36" s="100">
+      <c r="G36" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="100">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="51">
         <v>1</v>
       </c>
-      <c r="B37" s="100" t="s">
+      <c r="C37" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="D37" s="100">
+      <c r="E37" s="51">
         <v>2</v>
       </c>
-      <c r="E37" s="100">
+      <c r="F37" s="51">
         <v>2</v>
       </c>
-      <c r="F37" s="100">
+      <c r="G37" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="100">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="51">
         <v>2</v>
       </c>
-      <c r="B38" s="100" t="s">
+      <c r="C38" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="D38" s="100">
+      <c r="E38" s="51">
         <v>3</v>
       </c>
-      <c r="E38" s="100">
+      <c r="F38" s="51">
         <v>5</v>
       </c>
-      <c r="F38" s="100">
+      <c r="G38" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="100">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="51">
         <v>3</v>
       </c>
-      <c r="B39" s="100" t="s">
+      <c r="C39" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="D39" s="100">
+      <c r="E39" s="51">
         <v>4</v>
       </c>
-      <c r="E39" s="100">
+      <c r="F39" s="51">
         <v>2</v>
       </c>
-      <c r="F39" s="100">
+      <c r="G39" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="100">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="51">
         <v>4</v>
       </c>
-      <c r="B40" s="100" t="s">
+      <c r="C40" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="D40" s="100">
+      <c r="E40" s="51">
         <v>5</v>
       </c>
-      <c r="E40" s="100">
+      <c r="F40" s="51">
         <v>5</v>
       </c>
-      <c r="F40" s="100">
+      <c r="G40" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="100">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="51">
         <v>5</v>
       </c>
-      <c r="B41" s="100" t="s">
+      <c r="C41" s="51" t="s">
         <v>241</v>
       </c>
-      <c r="D41" s="100">
+      <c r="E41" s="51">
         <v>6</v>
       </c>
-      <c r="E41" s="100">
+      <c r="F41" s="51">
         <v>7</v>
       </c>
-      <c r="F41" s="100">
+      <c r="G41" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="98" t="s">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="E43" s="98" t="s">
+      <c r="F43" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="F43" s="98" t="s">
+      <c r="G43" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="100">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="51">
         <v>1</v>
       </c>
-      <c r="E44" s="100">
+      <c r="F44" s="51">
         <v>1</v>
       </c>
-      <c r="F44" s="100">
+      <c r="G44" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="100">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="51">
         <v>2</v>
       </c>
-      <c r="E45" s="100">
+      <c r="F45" s="51">
         <v>2</v>
       </c>
-      <c r="F45" s="100">
+      <c r="G45" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="100">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="51">
         <v>3</v>
       </c>
-      <c r="E46" s="100">
+      <c r="F46" s="51">
         <v>3</v>
       </c>
-      <c r="F46" s="100">
+      <c r="G46" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="100">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="51">
         <v>4</v>
       </c>
-      <c r="E47" s="100">
+      <c r="F47" s="51">
         <v>2</v>
       </c>
-      <c r="F47" s="100">
+      <c r="G47" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="100">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="51">
         <v>5</v>
       </c>
-      <c r="E48" s="100">
+      <c r="F48" s="51">
         <v>3</v>
       </c>
-      <c r="F48" s="100">
+      <c r="G48" s="51">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="98" t="s">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E50" s="49" t="s">
         <v>274</v>
       </c>
-      <c r="E50" s="98" t="s">
+      <c r="F50" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="F50" s="98" t="s">
+      <c r="G50" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="103" t="s">
+      <c r="H50" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="H50" s="103" t="s">
+      <c r="I50" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D51" s="100">
+    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E51" s="51">
         <v>1</v>
       </c>
-      <c r="E51" s="100" t="s">
+      <c r="F51" s="51" t="s">
         <v>275</v>
       </c>
-      <c r="F51" s="100">
+      <c r="G51" s="51">
         <v>1</v>
       </c>
-      <c r="G51" s="102">
+      <c r="H51" s="53">
         <v>45250</v>
       </c>
-      <c r="H51" s="102">
+      <c r="I51" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D52" s="100">
+    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E52" s="51">
         <v>2</v>
       </c>
-      <c r="E52" s="100" t="s">
+      <c r="F52" s="51" t="s">
         <v>276</v>
       </c>
-      <c r="F52" s="100">
+      <c r="G52" s="51">
         <v>1</v>
       </c>
-      <c r="G52" s="102">
+      <c r="H52" s="53">
         <v>45250</v>
       </c>
-      <c r="H52" s="102">
+      <c r="I52" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D53" s="100">
+    <row r="53" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E53" s="51">
         <v>3</v>
       </c>
-      <c r="E53" s="100" t="s">
+      <c r="F53" s="51" t="s">
         <v>277</v>
       </c>
-      <c r="F53" s="100">
+      <c r="G53" s="51">
         <v>2</v>
       </c>
-      <c r="G53" s="102">
+      <c r="H53" s="53">
         <v>45250</v>
       </c>
-      <c r="H53" s="102">
+      <c r="I53" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D55" s="98" t="s">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E55" s="49" t="s">
         <v>278</v>
       </c>
-      <c r="E55" s="98" t="s">
+      <c r="F55" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="F55" s="98" t="s">
+      <c r="G55" s="49" t="s">
         <v>279</v>
       </c>
-      <c r="G55" s="98" t="s">
+      <c r="H55" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="H55" s="98" t="s">
+      <c r="I55" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="103" t="s">
+      <c r="J55" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="J55" s="103" t="s">
+      <c r="K55" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D56" s="100">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E56" s="51">
         <v>1</v>
       </c>
-      <c r="E56" s="100" t="s">
+      <c r="F56" s="51" t="s">
         <v>280</v>
       </c>
-      <c r="F56" s="100">
+      <c r="G56" s="51">
         <v>5</v>
       </c>
-      <c r="G56" s="105">
+      <c r="H56" s="56">
         <v>1</v>
       </c>
-      <c r="H56" s="105">
+      <c r="I56" s="56">
         <v>1</v>
       </c>
-      <c r="I56" s="102">
+      <c r="J56" s="53">
         <v>45250</v>
       </c>
-      <c r="J56" s="102">
+      <c r="K56" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D57" s="100">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E57" s="51">
         <v>2</v>
       </c>
-      <c r="E57" s="100" t="s">
+      <c r="F57" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="F57" s="100">
+      <c r="G57" s="51">
         <v>0</v>
       </c>
-      <c r="G57" s="105">
+      <c r="H57" s="56">
         <v>2</v>
       </c>
-      <c r="H57" s="105">
+      <c r="I57" s="56">
         <v>2</v>
       </c>
-      <c r="I57" s="102">
+      <c r="J57" s="53">
         <v>45250</v>
       </c>
-      <c r="J57" s="102">
+      <c r="K57" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D59" s="98" t="s">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E59" s="49" t="s">
         <v>282</v>
       </c>
-      <c r="E59" s="98" t="s">
+      <c r="F59" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="F59" s="98" t="s">
+      <c r="G59" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="G59" s="98" t="s">
+      <c r="H59" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="H59" s="103" t="s">
+      <c r="I59" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="I59" s="103" t="s">
+      <c r="J59" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D60" s="100">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E60" s="51">
         <v>1</v>
       </c>
-      <c r="E60" s="100">
+      <c r="F60" s="51">
         <v>1</v>
       </c>
-      <c r="F60" s="100">
+      <c r="G60" s="51">
         <v>1</v>
       </c>
-      <c r="G60" s="100" t="s">
+      <c r="H60" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="H60" s="102">
+      <c r="I60" s="53">
         <v>45250</v>
       </c>
-      <c r="I60" s="102">
+      <c r="J60" s="53">
         <v>45250</v>
       </c>
     </row>
-    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D61" s="100">
+    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E61" s="51">
         <v>2</v>
       </c>
-      <c r="E61" s="100">
+      <c r="F61" s="51">
         <v>2</v>
       </c>
-      <c r="F61" s="100">
+      <c r="G61" s="51">
         <v>2</v>
       </c>
-      <c r="G61" s="100" t="s">
+      <c r="H61" s="51" t="s">
         <v>284</v>
       </c>
-      <c r="H61" s="102">
+      <c r="I61" s="53">
         <v>45250</v>
       </c>
-      <c r="I61" s="102">
+      <c r="J61" s="53">
         <v>45250</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{A873153E-40DB-41B6-8E2F-C71DC55AA566}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{206963B5-E983-4E50-8EF5-13FD7186C55D}"/>
-    <hyperlink ref="G16" r:id="rId3" xr:uid="{507B468B-04D3-4F87-85A1-5F47153D1EAE}"/>
-    <hyperlink ref="G17" r:id="rId4" xr:uid="{FA57DAA9-A7C8-43B0-81BA-1F2C49F02DDC}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{A873153E-40DB-41B6-8E2F-C71DC55AA566}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{206963B5-E983-4E50-8EF5-13FD7186C55D}"/>
+    <hyperlink ref="H16" r:id="rId3" xr:uid="{507B468B-04D3-4F87-85A1-5F47153D1EAE}"/>
+    <hyperlink ref="H17" r:id="rId4" xr:uid="{FA57DAA9-A7C8-43B0-81BA-1F2C49F02DDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6955,16 +6956,16 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="86" t="s">
+      <c r="G27" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="88"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="95"/>
+      <c r="M27" s="95"/>
+      <c r="N27" s="96"/>
       <c r="O27" s="9"/>
       <c r="P27" t="s">
         <v>43</v>
@@ -6975,14 +6976,14 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="91"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="99"/>
       <c r="O28" s="9"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
@@ -6990,14 +6991,14 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="94"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="101"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="102"/>
       <c r="O29" s="9"/>
     </row>
     <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7005,14 +7006,14 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="96"/>
-      <c r="J30" s="97"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="96"/>
-      <c r="N30" s="97"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="103"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="105"/>
       <c r="O30" s="9"/>
     </row>
     <row r="31" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>